<commit_message>
ccaa_t48 add large number of additional methods.
</commit_message>
<xml_diff>
--- a/utilityscripts/concrete/data/ccaa_t48_data.xlsx
+++ b/utilityscripts/concrete/data/ccaa_t48_data.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\concrete\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2488F21-EC11-46BA-8747-1BE2DDCFE6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F69583-6985-4BFE-BBF6-C85A4D839AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
   </bookViews>
   <sheets>
     <sheet name="w_fi_wheels" sheetId="1" r:id="rId1"/>
     <sheet name="w_fi_posts" sheetId="4" r:id="rId2"/>
     <sheet name="w_fi_distributed" sheetId="5" r:id="rId3"/>
+    <sheet name="e_sl_from_cbr" sheetId="6" r:id="rId4"/>
+    <sheet name="k_4" sheetId="7" r:id="rId5"/>
+    <sheet name="cht11_f_e1" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,12 +41,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>relative_depth</t>
   </si>
   <si>
     <t>w_fi</t>
+  </si>
+  <si>
+    <t>cbr</t>
+  </si>
+  <si>
+    <t>e_sl</t>
+  </si>
+  <si>
+    <t>f_c</t>
+  </si>
+  <si>
+    <t>k_4</t>
+  </si>
+  <si>
+    <t>e_ss</t>
+  </si>
+  <si>
+    <t>f_e1</t>
   </si>
 </sst>
 </file>
@@ -785,7 +806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD65B25D-74F4-4A7E-BDA0-A0A5BEE38177}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -953,4 +974,842 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E671C0-0B87-46E5-9678-EF71EC20B76D}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1.93514399541733</v>
+      </c>
+      <c r="B2" s="1">
+        <v>9.1549295774647899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>4.02619777864117</v>
+      </c>
+      <c r="B3" s="1">
+        <v>17.746478873239401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>4.8843996203230002</v>
+      </c>
+      <c r="B4" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>5.8780160722749102</v>
+      </c>
+      <c r="B5" s="1">
+        <v>22.112676056338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>7.7287967790701497</v>
+      </c>
+      <c r="B6" s="1">
+        <v>25.352112676056301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>9.7613635875767795</v>
+      </c>
+      <c r="B7" s="1">
+        <v>28.028169014084501</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>11.6528878421309</v>
+      </c>
+      <c r="B8" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>16.6065615805622</v>
+      </c>
+      <c r="B9" s="1">
+        <v>34.084507042253499</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>19.8245253140675</v>
+      </c>
+      <c r="B10" s="1">
+        <v>36.197183098591502</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>25.240496996036899</v>
+      </c>
+      <c r="B11" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>28.9426612471675</v>
+      </c>
+      <c r="B12" s="1">
+        <v>43.521126760563298</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>28.9426612471675</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43.521126760563298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>31.3692038539278</v>
+      </c>
+      <c r="B14" s="1">
+        <v>47.183098591549196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>33.1878425452485</v>
+      </c>
+      <c r="B15" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>39.301180392810501</v>
+      </c>
+      <c r="B16" s="1">
+        <v>59.8591549295774</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>46.540620354044997</v>
+      </c>
+      <c r="B17" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>55.559105469558297</v>
+      </c>
+      <c r="B18" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>65.793322465756702</v>
+      </c>
+      <c r="B19" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>73.643236559027201</v>
+      </c>
+      <c r="B20" s="1">
+        <v>96.338028169014095</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">
+    <sortCondition ref="A1:A20"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F762D2D-3DC2-4AAD-AB8C-45C0B9173E31}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>1.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AB0CFB-D570-4F1D-970D-0401B4E594ED}">
+  <dimension ref="A1:B72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3.55202295615514</v>
+      </c>
+      <c r="B2">
+        <v>0.80252164798861203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4.0979411868127604</v>
+      </c>
+      <c r="B3">
+        <v>0.84037536437590898</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4.6639367133060396</v>
+      </c>
+      <c r="B4">
+        <v>0.86044069237536502</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5.2137894807093197</v>
+      </c>
+      <c r="B5">
+        <v>0.88093782451179403</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5.9008469340084702</v>
+      </c>
+      <c r="B6">
+        <v>0.900423015524627</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6.6294605107390501</v>
+      </c>
+      <c r="B7">
+        <v>0.92000088103853195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7.4656095746560904</v>
+      </c>
+      <c r="B8">
+        <v>0.94059402495084998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8.3762828337628292</v>
+      </c>
+      <c r="B9">
+        <v>0.96007960990094598</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9.3221406289356903</v>
+      </c>
+      <c r="B10">
+        <v>0.98026345054557695</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10.491698223964599</v>
+      </c>
+      <c r="B11">
+        <v>1.00121285220791</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11.602675678526699</v>
+      </c>
+      <c r="B12">
+        <v>1.01947640254954</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12.8302345976005</v>
+      </c>
+      <c r="B13">
+        <v>1.03994390827682</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14.1738912965008</v>
+      </c>
+      <c r="B14">
+        <v>1.05954878750117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15.4591459683169</v>
+      </c>
+      <c r="B15">
+        <v>1.0792573782549699</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>17.0361328370279</v>
+      </c>
+      <c r="B16">
+        <v>1.1003706810990801</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>18.5842059897636</v>
+      </c>
+      <c r="B17">
+        <v>1.1201938652938199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>20.200594921304099</v>
+      </c>
+      <c r="B18">
+        <v>1.1396423556205999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>22.120966173590599</v>
+      </c>
+      <c r="B19">
+        <v>1.15994853787513</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>23.772524567090301</v>
+      </c>
+      <c r="B20">
+        <v>1.18006091450031</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>25.636720725665398</v>
+      </c>
+      <c r="B21">
+        <v>1.1999729500595999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>27.669363479074502</v>
+      </c>
+      <c r="B22">
+        <v>1.2202018081342201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>29.648768529821002</v>
+      </c>
+      <c r="B23">
+        <v>1.2397373849434801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>31.635083118982401</v>
+      </c>
+      <c r="B24">
+        <v>1.2593929115506699</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>33.762007859842299</v>
+      </c>
+      <c r="B25">
+        <v>1.2793849258935199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>36.113371611133701</v>
+      </c>
+      <c r="B26">
+        <v>1.29941416502408</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>38.398701253034602</v>
+      </c>
+      <c r="B27">
+        <v>1.3201299541288001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>41.104137049930202</v>
+      </c>
+      <c r="B28">
+        <v>1.33962273510456</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>43.954759141928498</v>
+      </c>
+      <c r="B29">
+        <v>1.3599986954910199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>47.109573971095699</v>
+      </c>
+      <c r="B30">
+        <v>1.3808399529611299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>49.9845754116104</v>
+      </c>
+      <c r="B31">
+        <v>1.39850544174004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>52.404594340712599</v>
+      </c>
+      <c r="B32">
+        <v>1.40816799070605</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>54.972472133057998</v>
+      </c>
+      <c r="B33">
+        <v>1.4170305701721</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>57.921419995880797</v>
+      </c>
+      <c r="B34">
+        <v>1.4253392595021901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>59.983247183165801</v>
+      </c>
+      <c r="B35">
+        <v>1.43015740135247</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>62.7062706270627</v>
+      </c>
+      <c r="B36">
+        <v>1.43536491373688</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>64.931984065986498</v>
+      </c>
+      <c r="B37">
+        <v>1.43867893742102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>67.491749174917501</v>
+      </c>
+      <c r="B38">
+        <v>1.44205845734274</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>69.880720948807195</v>
+      </c>
+      <c r="B39">
+        <v>1.4439510911092299</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>72.607260726072596</v>
+      </c>
+      <c r="B40">
+        <v>1.4460544258018599</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>74.911966082453006</v>
+      </c>
+      <c r="B41">
+        <v>1.44839006448015</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>78.045521447121899</v>
+      </c>
+      <c r="B42">
+        <v>1.4529323234185401</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>79.852260974448697</v>
+      </c>
+      <c r="B43">
+        <v>1.4566208236529701</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>82.829241828292496</v>
+      </c>
+      <c r="B44">
+        <v>1.46382206392856</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>84.973577266402501</v>
+      </c>
+      <c r="B45">
+        <v>1.46928475981672</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>87.9911952926103</v>
+      </c>
+      <c r="B46">
+        <v>1.4797825983187001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>89.922314149223098</v>
+      </c>
+      <c r="B47">
+        <v>1.48645467856604</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>92.396682590633404</v>
+      </c>
+      <c r="B48">
+        <v>1.4959004459013601</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>94.623526279568594</v>
+      </c>
+      <c r="B49">
+        <v>1.50681436725003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>96.457401774097804</v>
+      </c>
+      <c r="B50">
+        <v>1.51713196387897</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>98.243635805965695</v>
+      </c>
+      <c r="B51">
+        <v>1.52648449421196</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>99.935417405151398</v>
+      </c>
+      <c r="B52">
+        <v>1.5369989805425399</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>102.18866635521999</v>
+      </c>
+      <c r="B53">
+        <v>1.5512042206163601</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>104.755665064223</v>
+      </c>
+      <c r="B54">
+        <v>1.56506299368914</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>107.43054613680501</v>
+      </c>
+      <c r="B55">
+        <v>1.5798744341909401</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>109.784448764511</v>
+      </c>
+      <c r="B56">
+        <v>1.5905352581952401</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>112.010413370104</v>
+      </c>
+      <c r="B57">
+        <v>1.5997667961292601</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>114.94134002441299</v>
+      </c>
+      <c r="B58">
+        <v>1.61121620340967</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>117.326732673267</v>
+      </c>
+      <c r="B59">
+        <v>1.6201288018023301</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>119.76355169763499</v>
+      </c>
+      <c r="B60">
+        <v>1.6286496543797599</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>122.277227722772</v>
+      </c>
+      <c r="B61">
+        <v>1.6355783482539801</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>124.712288580456</v>
+      </c>
+      <c r="B62">
+        <v>1.6427495511615</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>127.39273927392701</v>
+      </c>
+      <c r="B63">
+        <v>1.64900545443765</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>129.99017938323499</v>
+      </c>
+      <c r="B64">
+        <v>1.6544751231952</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>132.343234323432</v>
+      </c>
+      <c r="B65">
+        <v>1.6590657793324199</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>135.02142451687999</v>
+      </c>
+      <c r="B66">
+        <v>1.66333164016303</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>137.62376237623701</v>
+      </c>
+      <c r="B67">
+        <v>1.6664285290804499</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>139.970161399701</v>
+      </c>
+      <c r="B68">
+        <v>1.6692862539473501</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>142.40924092409199</v>
+      </c>
+      <c r="B69">
+        <v>1.6711011146024699</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>144.945303543655</v>
+      </c>
+      <c r="B70">
+        <v>1.6722251931623</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>147.524752475247</v>
+      </c>
+      <c r="B71">
+        <v>1.67374977767237</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>150.092178167588</v>
+      </c>
+      <c r="B72">
+        <v>1.6746372247141801</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B72">
+    <sortCondition ref="A1:A72"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add helper data methods to allow excel reads to be cached.
</commit_message>
<xml_diff>
--- a/utilityscripts/concrete/data/ccaa_t48_data.xlsx
+++ b/utilityscripts/concrete/data/ccaa_t48_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\concrete\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F69583-6985-4BFE-BBF6-C85A4D839AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BE620B-D32E-4DF7-9FCA-D09270469226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
+    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
   </bookViews>
   <sheets>
     <sheet name="w_fi_wheels" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="e_sl_from_cbr" sheetId="6" r:id="rId4"/>
     <sheet name="k_4" sheetId="7" r:id="rId5"/>
     <sheet name="cht11_f_e1" sheetId="8" r:id="rId6"/>
+    <sheet name="cht12_f_e1" sheetId="9" r:id="rId7"/>
+    <sheet name="cht13_f_e1" sheetId="10" r:id="rId8"/>
+    <sheet name="cht14_f_e1" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>relative_depth</t>
   </si>
@@ -1224,7 +1227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AB0CFB-D570-4F1D-970D-0401B4E594ED}">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -1812,4 +1815,121 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD1F3D2-5535-478F-B12E-91D1BC08D30A}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2756CE3D-CA0B-49BC-927E-820826FB3317}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4FF09A-ECDC-4607-B00C-BBA37F8F7346}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CCAA T48 add data for f_e2
</commit_message>
<xml_diff>
--- a/utilityscripts/concrete/data/ccaa_t48_data.xlsx
+++ b/utilityscripts/concrete/data/ccaa_t48_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\concrete\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BE620B-D32E-4DF7-9FCA-D09270469226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C67B58-FEBE-42AA-8F36-F8742D13EE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-270" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="5" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
   </bookViews>
   <sheets>
     <sheet name="w_fi_wheels" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,14 @@
     <sheet name="w_fi_distributed" sheetId="5" r:id="rId3"/>
     <sheet name="e_sl_from_cbr" sheetId="6" r:id="rId4"/>
     <sheet name="k_4" sheetId="7" r:id="rId5"/>
-    <sheet name="cht11_f_e1" sheetId="8" r:id="rId6"/>
-    <sheet name="cht12_f_e1" sheetId="9" r:id="rId7"/>
-    <sheet name="cht13_f_e1" sheetId="10" r:id="rId8"/>
-    <sheet name="cht14_f_e1" sheetId="11" r:id="rId9"/>
+    <sheet name="cht11_f_e" sheetId="8" r:id="rId6"/>
+    <sheet name="cht11_f_s" sheetId="12" r:id="rId7"/>
+    <sheet name="cht12_f_e" sheetId="9" r:id="rId8"/>
+    <sheet name="cht12_f_s" sheetId="13" r:id="rId9"/>
+    <sheet name="cht13_f_e" sheetId="10" r:id="rId10"/>
+    <sheet name="cht13_f_s" sheetId="14" r:id="rId11"/>
+    <sheet name="cht14_f_e" sheetId="11" r:id="rId12"/>
+    <sheet name="cht14_f_s" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
   <si>
     <t>relative_depth</t>
   </si>
@@ -67,7 +71,13 @@
     <t>e_ss</t>
   </si>
   <si>
-    <t>f_e1</t>
+    <t>x</t>
+  </si>
+  <si>
+    <t>f_e</t>
+  </si>
+  <si>
+    <t>f_s</t>
   </si>
 </sst>
 </file>
@@ -631,6 +641,162 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2756CE3D-CA0B-49BC-927E-820826FB3317}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA43ABBA-596A-44DB-ACD5-DD0354E71F86}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>0.999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4FF09A-ECDC-4607-B00C-BBA37F8F7346}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D80BD14-9AEF-4A12-BFA1-6D4BF756A2E8}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>0.999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B6098F-5767-4F6A-BECF-496C16DDDEC6}">
   <dimension ref="A1:B19"/>
@@ -1227,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AB0CFB-D570-4F1D-970D-0401B4E594ED}">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,7 +1404,7 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1818,37 +1984,357 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD1F3D2-5535-478F-B12E-91D1BC08D30A}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFACA784-0983-40FB-92BC-3B6D32F86921}">
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD72"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" s="1">
+        <v>0.90023014452141803</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>100</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
+      <c r="A3" s="1">
+        <v>1.0462753950338599</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.91056433408577797</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1.0880361173814801</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.92020990633351496</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1.1331828442437899</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.93031447030435099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1.1828442437923199</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.94041799641939705</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1.2505643340857699</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.95419553203082397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1.3002257336343099</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.96429905814587002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1.3498871331828399</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.97417269920344496</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1.4018058690744899</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.98312628110323996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1.4492099322798999</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.99185101580135404</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1.5011286681715501</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.0010344827586199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1.5507900677200901</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.00952881347136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1.6004514672686201</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.0175633740691701</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1.6501128668171501</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0255979346669699</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1.6997742663656801</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.03363249526478</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>1.7494356659142201</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.04097740069017</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>1.80135440180586</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0492413274175501</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1.8510158013544</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.056126462728</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>1.90067720090293</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.06278171298098</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>1.95033860045146</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.06943696323395</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.0763220985444</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>2.0496613995485302</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.0827474637399099</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>2.09932279909706</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.0887130588204701</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>2.1489841986455902</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1.09467865390104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>2.1986455981941302</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1.1001844788666599</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>2.2505643340857699</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1.1056897849043801</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>2.2979683972911902</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1.1111961287979</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>2.3498871331828401</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.1162416647206801</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>2.3995485327313699</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1.12128771957136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>2.4514672686230199</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.1261033704366701</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>2.5011286681715501</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1.1309195402298799</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>2.5507900677200901</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1.13504605485067</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>2.6004514672686199</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1.1391725694714701</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>2.6523702031602698</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1.1432985651643699</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>2.6997742663656799</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1.1471957136555799</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>2.75395033860045</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1.15063153524817</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>2.80135440180586</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1.15429879868192</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>2.8555304740406302</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1.15773462027451</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>2.9029345372460398</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1.1602524584209</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>2.9525959367945802</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1.1629996626968599</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>2.9954853273137698</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1.1657484237565101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>3</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1.1659772709581999</v>
       </c>
     </row>
   </sheetData>
@@ -1857,76 +2343,392 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2756CE3D-CA0B-49BC-927E-820826FB3317}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD1F3D2-5535-478F-B12E-91D1BC08D30A}">
+  <dimension ref="A1:B42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>4.0404040404040398</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.801681957186544</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>5.0505050505050502</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.85382262996941904</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>6.3973063973063899</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.90091743119265999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>7.7441077441077404</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.93960244648318003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>9.2592592592592595</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.98165137614678899</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>11.4478114478114</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.0321100917431101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>13.973063973063899</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.08425076452599</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>16.498316498316498</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.13302752293577</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>19.360269360269299</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.17675840978593</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>22.5589225589225</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.2204892966360801</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>25.252525252525199</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.25581039755351</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>28.1144781144781</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.2894495412844</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>31.481481481481399</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.3281345565749201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>35.858585858585798</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.3718654434250701</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>39.5622895622895</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.4071865443425</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>42.929292929292899</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.4357798165137601</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45.959595959595902</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.4593272171253799</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>49.494949494949402</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.4862385321100899</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>53.872053872053797</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.5114678899082501</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>58.417508417508401</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.5333333333333301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>63.636363636363598</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.5501529051987699</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>68.855218855218794</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.56360856269113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>74.579124579124496</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.5703363914373001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>79.292929292929301</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1.5770642201834799</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>83.501683501683502</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1.5854740061162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>86.700336700336706</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1.5972477064220101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>90.2356902356902</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1.61238532110091</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>93.771043771043693</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.6308868501528999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>97.138047138047099</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1.6561162079510701</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>100.84175084175</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.6880733944954101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>104.208754208754</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1.72003058103975</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>108.080808080808</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1.75198776758409</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>111.952861952861</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1.7755351681957099</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>116.666666666666</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1.80076452599388</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>121.717171717171</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1.8243119266054999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>126.59932659932601</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1.8411314984709399</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>130.47138047138</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1.85290519877675</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>135.18518518518499</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1.8613149847094801</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>139.89898989898899</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1.8714067278287401</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>144.78114478114401</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1.8764525993883701</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>150</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1.88149847094801</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0FCA13A-08B5-4A81-B7EB-363371A4C292}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" s="1">
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>100</v>
       </c>
       <c r="B3">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4FF09A-ECDC-4607-B00C-BBA37F8F7346}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>100</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
+        <v>0.999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ccaa_t48 add f_s2 data.
</commit_message>
<xml_diff>
--- a/utilityscripts/concrete/data/ccaa_t48_data.xlsx
+++ b/utilityscripts/concrete/data/ccaa_t48_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\concrete\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C67B58-FEBE-42AA-8F36-F8742D13EE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC29C13F-EA50-411B-AE6B-730C0C2B8C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="5" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
   </bookViews>
   <sheets>
     <sheet name="w_fi_wheels" sheetId="1" r:id="rId1"/>
@@ -1393,7 +1393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21AB0CFB-D570-4F1D-970D-0401B4E594ED}">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -2699,13 +2699,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0FCA13A-08B5-4A81-B7EB-363371A4C292}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2720,15 +2723,247 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0.1</v>
+        <v>0.91425269645608598</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>100</v>
-      </c>
-      <c r="B3">
-        <v>0.999</v>
+        <v>1.0475651189127899</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.92619414483821205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1.0679501698754199</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.93043143297380504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1.0973952434881</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.93736517719568502</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1.1472253680634199</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.94699537750385199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1.19705549263873</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.95624036979969096</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1.2468856172140399</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.96625577812018404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1.29671574178935</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.97473035439137101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1.3488108720271801</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.98320493066255699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1.4009060022649999</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.99129429892141696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1.4484711211778001</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.99822804314329705</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1.49830124575311</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.0055469953775</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1.55039637599094</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.0120955315870499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1.6002265005662499</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.01941448382126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1.65005662514156</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0251926040061601</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>1.6998867497168699</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.03174114021571</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>1.74971687429218</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0371340523882799</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1.7995469988674899</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.04291217257318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>1.8810872027179999</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.05138674884437</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>1.96715741789354</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.0602465331278801</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>2.0509626274065602</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.0675654853620899</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>2.14835787089467</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.0760400616332799</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>2.2321630804077</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.08258859784283</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>2.3227633069082598</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1.0899075500770401</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>2.4201585503963701</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1.09645608628659</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>2.5016987542468798</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1.10184899845916</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>2.6013590033975</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1.10762711864406</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>2.6761041902604701</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.1118644067796599</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>2.7848244620611502</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1.1172573189522299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>2.90033975084937</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.1226502311247999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>3</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1.1268875192604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ccaa t48 updated _s3
</commit_message>
<xml_diff>
--- a/utilityscripts/concrete/data/ccaa_t48_data.xlsx
+++ b/utilityscripts/concrete/data/ccaa_t48_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\concrete\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC29C13F-EA50-411B-AE6B-730C0C2B8C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F62DE5C-7656-4D8E-BF05-62D39B150F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" firstSheet="3" activeTab="10" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
   </bookViews>
   <sheets>
     <sheet name="w_fi_wheels" sheetId="1" r:id="rId1"/>
@@ -682,13 +682,16 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA43ABBA-596A-44DB-ACD5-DD0354E71F86}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -703,15 +706,239 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0.1</v>
+        <v>0.71054263565891396</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>100</v>
-      </c>
-      <c r="B3">
-        <v>0.999</v>
+        <v>1.0250855188141299</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.74775193798449602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1.0250855188141299</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.74775193798449602</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1.0490307867730899</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.78248062015503805</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1.0752565564424099</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.81596899224806196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1.1094640820980599</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.85813953488371997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1.1436716077536999</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.90031007751937897</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1.17331812998859</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.93379844961240299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1.2006841505131101</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.96480620155038699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1.2497149372862</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.01751937984496</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1.22576966932725</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.99271317829457295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1.2884834663625899</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.0565891472868201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1.32155074116305</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.08883720930232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1.3534777651083201</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.1186046511627901</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1.3842645381984</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.1458914728682099</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>1.41619156214367</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.17317829457364</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>1.45039908779931</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.2017054263565801</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1.49258836944127</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.23395348837209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>1.5302166476624799</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.26248062015503</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>1.56784492588369</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.2872868217054201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>1.6088939566704601</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.31395348837209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>1.6510832383124201</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.34062015503875</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>1.69783352337514</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.36666666666666</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>1.7400228050171</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1.38775193798449</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>1.77651083238312</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1.40511627906976</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>1.8198403648802699</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1.42372093023255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>1.8677309007981699</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1.44232558139534</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>1.9144811858608799</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.4572093023255801</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>1.95496009122006</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1.4689922480620099</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.4807751937984399</v>
       </c>
     </row>
   </sheetData>
@@ -2701,7 +2928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0FCA13A-08B5-4A81-B7EB-363371A4C292}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ccaa t48 - finish updating f_e and f_s
</commit_message>
<xml_diff>
--- a/utilityscripts/concrete/data/ccaa_t48_data.xlsx
+++ b/utilityscripts/concrete/data/ccaa_t48_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\concrete\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F62DE5C-7656-4D8E-BF05-62D39B150F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6610007-7963-4CD0-AB38-8BD7BFD0550F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" firstSheet="3" activeTab="10" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="13" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
   </bookViews>
   <sheets>
     <sheet name="w_fi_wheels" sheetId="1" r:id="rId1"/>
@@ -22,10 +22,11 @@
     <sheet name="cht11_f_s" sheetId="12" r:id="rId7"/>
     <sheet name="cht12_f_e" sheetId="9" r:id="rId8"/>
     <sheet name="cht12_f_s" sheetId="13" r:id="rId9"/>
-    <sheet name="cht13_f_e" sheetId="10" r:id="rId10"/>
-    <sheet name="cht13_f_s" sheetId="14" r:id="rId11"/>
-    <sheet name="cht14_f_e" sheetId="11" r:id="rId12"/>
-    <sheet name="cht14_f_s" sheetId="15" r:id="rId13"/>
+    <sheet name="cht13_f_e_interior" sheetId="10" r:id="rId10"/>
+    <sheet name="cht13_f_e_edge" sheetId="16" r:id="rId11"/>
+    <sheet name="cht13_f_s" sheetId="14" r:id="rId12"/>
+    <sheet name="cht14_f_e" sheetId="11" r:id="rId13"/>
+    <sheet name="cht14_f_s" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
   <si>
     <t>relative_depth</t>
   </si>
@@ -643,10 +644,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2756CE3D-CA0B-49BC-927E-820826FB3317}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,31 +662,544 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2.8653295128939802</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.59825934584661</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>100</v>
+        <v>4.5845272206303704</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>0.67718375210652804</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6.1891117478510003</v>
+      </c>
+      <c r="B4">
+        <v>0.73551631807392404</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7.9083094555873901</v>
+      </c>
+      <c r="B5">
+        <v>0.79556396926363904</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>9.2836676217765</v>
+      </c>
+      <c r="B6">
+        <v>0.84016995292992003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10.8882521489971</v>
+      </c>
+      <c r="B7">
+        <v>0.88649003839809504</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>12.378223495702001</v>
+      </c>
+      <c r="B8">
+        <v>0.924230764072968</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>14.0974212034383</v>
+      </c>
+      <c r="B9">
+        <v>0.96883379747797105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>14.0974212034383</v>
+      </c>
+      <c r="B10">
+        <v>0.96883379747797105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>15.702005730659</v>
+      </c>
+      <c r="B11">
+        <v>1.01000567701791</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>18.4527220630372</v>
+      </c>
+      <c r="B12">
+        <v>1.0614641342100599</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>21.6618911174785</v>
+      </c>
+      <c r="B13">
+        <v>1.1163507950060101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>24.527220630372501</v>
+      </c>
+      <c r="B14">
+        <v>1.1626600628495001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>27.736389684813702</v>
+      </c>
+      <c r="B15">
+        <v>1.2141145863599501</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>30.487106017191898</v>
+      </c>
+      <c r="B16">
+        <v>1.2569927003383801</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>34.040114613180499</v>
+      </c>
+      <c r="B17">
+        <v>1.3067282049448099</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>37.478510028653297</v>
+      </c>
+      <c r="B18">
+        <v>1.35474862432892</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>41.833810888252103</v>
+      </c>
+      <c r="B19">
+        <v>1.4096254509206101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>47.220630372492799</v>
+      </c>
+      <c r="B20">
+        <v>1.4644934267284699</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>49.169054441260698</v>
+      </c>
+      <c r="B21">
+        <v>1.4816373950086901</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>51.346704871060098</v>
+      </c>
+      <c r="B22">
+        <v>1.49877939644806</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>53.295128939827997</v>
+      </c>
+      <c r="B23">
+        <v>1.51077515880004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>55.128939828080199</v>
+      </c>
+      <c r="B24">
+        <v>1.5210558359297099</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>59.140401146131801</v>
+      </c>
+      <c r="B25">
+        <v>1.53818210264227</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>63.037249283667599</v>
+      </c>
+      <c r="B26">
+        <v>1.5570254214179999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>66.532951289398198</v>
+      </c>
+      <c r="B27">
+        <v>1.57072397623698</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>71.404011461318007</v>
+      </c>
+      <c r="B28">
+        <v>1.58784286729635</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>79.426934097421196</v>
+      </c>
+      <c r="B29">
+        <v>1.6152311261504899</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>84.011461318051502</v>
+      </c>
+      <c r="B30">
+        <v>1.6272042698326801</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>89.856733524355306</v>
+      </c>
+      <c r="B31">
+        <v>1.6443148018184299</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>95.931232091690504</v>
+      </c>
+      <c r="B32">
+        <v>1.66313943560607</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>100.057306590257</v>
+      </c>
+      <c r="B33">
+        <v>1.6751165129699701</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B33">
+    <sortCondition ref="A2:A33"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1189659-55E8-4E76-8A86-E883731015EF}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>2.8653295128939802</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.59825934584661</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>4.5845272206303704</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.67718375210652804</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>6.1891117478510003</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.73551631807392404</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>7.9083094555873901</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.79556396926363904</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>9.2836676217765</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.84016995292992003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>10.8882521489971</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.88649003839809504</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>12.378223495702001</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.924230764072968</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>14.0974212034383</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.96883379747797105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>14.0974212034383</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.96883379747797105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>16.160458452722001</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.0014214001224699</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>18.3381088825214</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.0357240879892999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>20.859598853868199</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.06659168830936</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>23.7249283667621</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.1034625786177501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>26.934097421203401</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.14376265595036</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>30.945558739254999</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.1934942268750901</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>34.4985673352435</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.23293331962504</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>38.166189111747798</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.27065536031183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>41.489971346704799</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.30323214533165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>45.157593123209097</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.33752204873295</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>50.085959885386799</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.37008506586681</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>55.014326647564403</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.3923516711442001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>60.057306590257802</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.41118515571568</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>64.985673352435498</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.42487141777934</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>70.028653295128905</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1.44027276506532</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>75.186246418338101</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1.45395706028814</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>80</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1.46421216848673</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>85.157593123209097</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1.47789646370955</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>89.971346704870996</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.4898676405508899</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>95.014326647564403</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1.50012078190863</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>100</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.5103744149765901</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B31">
+    <sortCondition ref="A1:A31"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA43ABBA-596A-44DB-ACD5-DD0354E71F86}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,18 +1289,18 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1.2497149372862</v>
+        <v>1.22576966932725</v>
       </c>
       <c r="B11" s="1">
-        <v>1.01751937984496</v>
+        <v>0.99271317829457295</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1.22576966932725</v>
+        <v>1.2497149372862</v>
       </c>
       <c r="B12" s="1">
-        <v>0.99271317829457295</v>
+        <v>1.01751937984496</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -942,16 +1456,19 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B31">
+    <sortCondition ref="A2:A31"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4FF09A-ECDC-4607-B00C-BBA37F8F7346}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,31 +1483,210 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>4.1189931350114302</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.49991465437687599</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>100</v>
+        <v>5.7494279176201299</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>0.61176898362251098</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8.3237986270022795</v>
+      </c>
+      <c r="B4">
+        <v>0.72981976071218901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10.383295194507999</v>
+      </c>
+      <c r="B5">
+        <v>0.82923318735673801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>13.4725400457665</v>
+      </c>
+      <c r="B6">
+        <v>0.94727329624352896</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>16.3901601830663</v>
+      </c>
+      <c r="B7">
+        <v>1.04666894254993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>20.680778032036599</v>
+      </c>
+      <c r="B8">
+        <v>1.1895481838273401</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>24.284897025171599</v>
+      </c>
+      <c r="B9">
+        <v>1.29514561207923</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>28.060640732265401</v>
+      </c>
+      <c r="B10">
+        <v>1.4069554904795001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>32.179633867276799</v>
+      </c>
+      <c r="B11">
+        <v>1.5249742629605101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>35.955377574370701</v>
+      </c>
+      <c r="B12">
+        <v>1.6243521289287699</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>41.962242562928999</v>
+      </c>
+      <c r="B13">
+        <v>1.7858438281779101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>49.170480549198999</v>
+      </c>
+      <c r="B14">
+        <v>1.9597426473856501</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>56.378718535469098</v>
+      </c>
+      <c r="B15">
+        <v>2.1460734790254099</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>64.788329519450798</v>
+      </c>
+      <c r="B16">
+        <v>2.34481143062377</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>74.914187643020597</v>
+      </c>
+      <c r="B17">
+        <v>2.5870258650578899</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>84.696796338672698</v>
+      </c>
+      <c r="B18">
+        <v>2.82303140541126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>94.822654462242497</v>
+      </c>
+      <c r="B19">
+        <v>3.05902983362936</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>104.948512585812</v>
+      </c>
+      <c r="B20">
+        <v>3.2950282618474702</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>114.902745995423</v>
+      </c>
+      <c r="B21">
+        <v>3.52792224302521</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>124.68535469107501</v>
+      </c>
+      <c r="B22">
+        <v>3.7546037740545701</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>134.98283752860399</v>
+      </c>
+      <c r="B23">
+        <v>3.9905986462050498</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>145.108695652173</v>
+      </c>
+      <c r="B24">
+        <v>4.2203810682071499</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>150</v>
+      </c>
+      <c r="B25">
+        <v>4.33527583527583</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B25">
+    <sortCondition ref="A2:A25"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D80BD14-9AEF-4A12-BFA1-6D4BF756A2E8}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,18 +1701,258 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0.98879551820728195</v>
       </c>
       <c r="B2" s="1">
-        <v>0.1</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>100</v>
-      </c>
-      <c r="B3">
-        <v>0.999</v>
+        <v>1.0138235722423501</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.6415137614678801</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1.03609976100531</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.59885321100917</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1.0695461670906801</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.5451834862385301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1.10582367503576</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.5011467889908201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1.1644715990371599</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.4447247706422</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1.22314950445009</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.39793577981651</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1.30420639203693</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.34151376146788</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1.3797038693153001</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.29885321100917</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1.48319541884031</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.2506880733944901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1.59789573321683</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.2038990825688001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1.7098206254979</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.1653669724770599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1.8441501983056201</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.12545871559633</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1.9952907768612</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0869266055045801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>2.1296503310804402</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.05665137614678</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>2.2612258970866601</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.0318807339449501</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>2.4404033784767698</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0016055045871499</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>2.6307981908359599</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.97545871559632902</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>2.7820072983321702</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.95894495412843905</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>2.9220162070944502</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.94380733944953998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>3.0956342781760999</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.92729357798165102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>3.27766427671986</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.91353211009174196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>3.4765074225408799</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.90183486238531996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>3.6501511919752598</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.89357798165137503</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>3.8406016840987101</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.88532110091742999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>4.0198584020764203</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.88050458715596303</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>4.1823191050120299</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.87912844036697202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>4.39520425907366</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.87912844036697202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>4.5800889163004603</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.88256880733944898</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>4.7649842811742404</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.88944954128440301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>4.8938636616726203</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.898394495412843</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>4.99753509966677</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.90802752293577904</v>
       </c>
     </row>
   </sheetData>
@@ -1621,7 +2557,7 @@
   <dimension ref="A1:B72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="A2" sqref="A2:B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,7 +3140,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B72">
-    <sortCondition ref="A1:A72"/>
+    <sortCondition ref="A2:A72"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2214,8 +3150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFACA784-0983-40FB-92BC-3B6D32F86921}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A43" sqref="A2:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2565,6 +3501,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B43">
+    <sortCondition ref="A43"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2574,7 +3513,7 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2920,6 +3859,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B42">
+    <sortCondition ref="A2:A42"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2929,7 +3871,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3194,6 +4136,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B32">
+    <sortCondition ref="A2:A32"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ccaa t48 fix error in data add plot for f_s
</commit_message>
<xml_diff>
--- a/utilityscripts/concrete/data/ccaa_t48_data.xlsx
+++ b/utilityscripts/concrete/data/ccaa_t48_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\concrete\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6610007-7963-4CD0-AB38-8BD7BFD0550F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D546C4-0F10-4CF3-BA36-DE6476F0ABE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="13" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="14" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
   </bookViews>
   <sheets>
     <sheet name="w_fi_wheels" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,17 @@
     <sheet name="k_4" sheetId="7" r:id="rId5"/>
     <sheet name="cht11_f_e" sheetId="8" r:id="rId6"/>
     <sheet name="cht11_f_s" sheetId="12" r:id="rId7"/>
-    <sheet name="cht12_f_e" sheetId="9" r:id="rId8"/>
-    <sheet name="cht12_f_s" sheetId="13" r:id="rId9"/>
-    <sheet name="cht13_f_e_interior" sheetId="10" r:id="rId10"/>
-    <sheet name="cht13_f_e_edge" sheetId="16" r:id="rId11"/>
-    <sheet name="cht13_f_s" sheetId="14" r:id="rId12"/>
-    <sheet name="cht14_f_e" sheetId="11" r:id="rId13"/>
-    <sheet name="cht14_f_s" sheetId="15" r:id="rId14"/>
+    <sheet name="cht11_f_h" sheetId="17" r:id="rId8"/>
+    <sheet name="cht12_f_e" sheetId="9" r:id="rId9"/>
+    <sheet name="cht12_f_s" sheetId="13" r:id="rId10"/>
+    <sheet name="cht12_f_h" sheetId="18" r:id="rId11"/>
+    <sheet name="cht13_f_e_interior" sheetId="10" r:id="rId12"/>
+    <sheet name="cht13_f_e_edge" sheetId="16" r:id="rId13"/>
+    <sheet name="cht13_f_s" sheetId="14" r:id="rId14"/>
+    <sheet name="cht13_f_h" sheetId="19" r:id="rId15"/>
+    <sheet name="cht14_f_e" sheetId="11" r:id="rId16"/>
+    <sheet name="cht14_f_s" sheetId="15" r:id="rId17"/>
+    <sheet name="cht14_f_h" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
   <si>
     <t>relative_depth</t>
   </si>
@@ -79,6 +83,12 @@
   </si>
   <si>
     <t>f_s</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>f_h</t>
   </si>
 </sst>
 </file>
@@ -643,6 +653,326 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0FCA13A-08B5-4A81-B7EB-363371A4C292}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.91425269645608598</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1.0475651189127899</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.92619414483821205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1.0679501698754199</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.93043143297380504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1.0973952434881</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.93736517719568502</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1.1472253680634199</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.94699537750385199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1.19705549263873</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.95624036979969096</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1.2468856172140399</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.96625577812018404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1.29671574178935</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.97473035439137101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1.3488108720271801</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.98320493066255699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1.4009060022649999</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.99129429892141696</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1.4484711211778001</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.99822804314329705</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1.49830124575311</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.0055469953775</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1.55039637599094</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.0120955315870499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1.6002265005662499</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.01941448382126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1.65005662514156</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0251926040061601</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>1.6998867497168699</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.03174114021571</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>1.74971687429218</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0371340523882799</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1.7995469988674899</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.04291217257318</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>1.8810872027179999</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.05138674884437</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>1.96715741789354</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.0602465331278801</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>2.0509626274065602</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.0675654853620899</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>2.14835787089467</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.0760400616332799</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>2.2321630804077</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.08258859784283</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>2.3227633069082598</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1.0899075500770401</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>2.4201585503963701</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1.09645608628659</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>2.5016987542468798</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1.10184899845916</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>2.6013590033975</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1.10762711864406</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>2.6761041902604701</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1.1118644067796599</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>2.7848244620611502</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1.1172573189522299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>2.90033975084937</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.1226502311247999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>3</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1.1268875192604</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B32">
+    <sortCondition ref="A2:A32"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04344E26-F4EF-4CD8-95B7-38818E26435E}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2756CE3D-CA0B-49BC-927E-820826FB3317}">
   <dimension ref="A1:B33"/>
   <sheetViews>
@@ -924,7 +1254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1189659-55E8-4E76-8A86-E883731015EF}">
   <dimension ref="A1:B31"/>
   <sheetViews>
@@ -1194,17 +1524,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA43ABBA-596A-44DB-ACD5-DD0354E71F86}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B31"/>
+      <selection activeCell="B2" sqref="B2:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1217,253 +1548,272 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="B2" s="1">
-        <v>0.71054263565891396</v>
+        <v>0.71054263565891496</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1.0250855188141299</v>
+        <v>1.04905875641756</v>
       </c>
       <c r="B3" s="1">
-        <v>0.74775193798449602</v>
+        <v>0.74897703604452204</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1.0250855188141299</v>
+        <v>1.1266400456360499</v>
       </c>
       <c r="B4" s="1">
-        <v>0.74775193798449602</v>
+        <v>0.79980569300910498</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1.0490307867730899</v>
+        <v>1.19965772960638</v>
       </c>
       <c r="B5" s="1">
-        <v>0.78248062015503805</v>
+        <v>0.84567452473500604</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>1.0752565564424099</v>
+        <v>1.2703936109526499</v>
       </c>
       <c r="B6" s="1">
-        <v>0.81596899224806196</v>
+        <v>0.89030375391908401</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>1.1094640820980599</v>
+        <v>1.34569309754706</v>
       </c>
       <c r="B7" s="1">
-        <v>0.85813953488371997</v>
+        <v>0.93369125795424901</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>1.1436716077536999</v>
+        <v>1.4209925841414699</v>
       </c>
       <c r="B8" s="1">
-        <v>0.90031007751937897</v>
+        <v>0.975838451911894</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>1.17331812998859</v>
+        <v>1.4917284654877301</v>
       </c>
       <c r="B9" s="1">
-        <v>0.93379844961240299</v>
+        <v>1.01302582063085</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1.2006841505131101</v>
+        <v>1.5510553337136299</v>
       </c>
       <c r="B10" s="1">
-        <v>0.96480620155038699</v>
+        <v>1.0440151766407</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1.22576966932725</v>
+        <v>1.6354820308043301</v>
       </c>
       <c r="B11" s="1">
-        <v>0.99271317829457295</v>
+        <v>1.0849192303780399</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1.2497149372862</v>
+        <v>1.7153451226468901</v>
       </c>
       <c r="B12" s="1">
-        <v>1.01751937984496</v>
+        <v>1.1221037689542099</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1.2884834663625899</v>
+        <v>1.7860810039931501</v>
       </c>
       <c r="B13" s="1">
-        <v>1.0565891472868201</v>
+        <v>1.1543298973631</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1.32155074116305</v>
+        <v>1.8454078722190499</v>
       </c>
       <c r="B14" s="1">
-        <v>1.08883720930232</v>
+        <v>1.1791177029853499</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1.3534777651083201</v>
+        <v>1.9526525955504801</v>
       </c>
       <c r="B15" s="1">
-        <v>1.1186046511627901</v>
+        <v>1.22249530152075</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1.3842645381984</v>
+        <v>2.02795208214489</v>
       </c>
       <c r="B16" s="1">
-        <v>1.1458914728682099</v>
+        <v>1.24975877454817</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>1.41619156214367</v>
+        <v>2.10096976611523</v>
       </c>
       <c r="B17" s="1">
-        <v>1.17317829457364</v>
+        <v>1.2757826450337599</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1.45039908779931</v>
+        <v>2.18083285795778</v>
       </c>
       <c r="B18" s="1">
-        <v>1.2017054263565801</v>
+        <v>1.30180439291226</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1.49258836944127</v>
+        <v>2.2538505419281201</v>
       </c>
       <c r="B19" s="1">
-        <v>1.23395348837209</v>
+        <v>1.32534764324281</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>1.5302166476624799</v>
+        <v>2.35196805476326</v>
       </c>
       <c r="B20" s="1">
-        <v>1.26248062015503</v>
+        <v>1.3538443509907701</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>1.56784492588369</v>
+        <v>2.4181403308613798</v>
       </c>
       <c r="B21" s="1">
-        <v>1.2872868217054201</v>
+        <v>1.37242848361833</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1.6088939566704601</v>
+        <v>2.5208214489446599</v>
       </c>
       <c r="B22" s="1">
-        <v>1.31395348837209</v>
+        <v>1.39720284606234</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1.6510832383124201</v>
+        <v>2.6212207644038701</v>
       </c>
       <c r="B23" s="1">
-        <v>1.34062015503875</v>
+        <v>1.419497295887</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>1.69783352337514</v>
+        <v>2.7375926982315999</v>
       </c>
       <c r="B24" s="1">
-        <v>1.36666666666666</v>
+        <v>1.44054648288426</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>1.7400228050171</v>
+        <v>2.8357102110667398</v>
       </c>
       <c r="B25" s="1">
-        <v>1.38775193798449</v>
+        <v>1.45664008985703</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>1.77651083238312</v>
+        <v>2.89960068454078</v>
       </c>
       <c r="B26" s="1">
-        <v>1.40511627906976</v>
+        <v>1.4665427594776601</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1.8198403648802699</v>
+        <v>2.9680547632629701</v>
       </c>
       <c r="B27" s="1">
-        <v>1.42372093023255</v>
+        <v>1.4752037039493699</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>1.8677309007981699</v>
+        <v>3</v>
       </c>
       <c r="B28" s="1">
-        <v>1.44232558139534</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>1.9144811858608799</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1.4572093023255801</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>1.95496009122006</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1.4689922480620099</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>2</v>
-      </c>
-      <c r="B31" s="1">
-        <v>1.4807751937984399</v>
+        <v>1.4795348837209199</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B31">
-    <sortCondition ref="A2:A31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B5">
+    <sortCondition ref="A2:A5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B904222-846F-4A0A-B02A-B94E3C0047B2}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4FF09A-ECDC-4607-B00C-BBA37F8F7346}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -1681,11 +2031,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D80BD14-9AEF-4A12-BFA1-6D4BF756A2E8}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B33"/>
     </sheetView>
   </sheetViews>
@@ -1953,6 +2303,49 @@
       </c>
       <c r="B33" s="1">
         <v>0.90802752293577904</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D2C553-794E-4F5B-8849-B0EB72C79CE0}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.2</v>
       </c>
     </row>
   </sheetData>
@@ -3509,6 +3902,284 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EC66B3-8A02-4357-A7CE-EE0CCC9AA465}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0.402810304449639</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0.53395784543324598</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.2716973578863</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.71194379391099805</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.2380704563650899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.87119437939109201</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.2094875900720501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1.0023419203746899</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.18763010408326</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1.1334894613583</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.1680144115292199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1.30210772833722</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.1472778222578</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1.49882903981263</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.1226180944755799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1.7236533957845299</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.10076060848678</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>2.05152224824355</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.0744195356285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>2.3887587822013998</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.0570456365092</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>2.7259953161592398</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.04079263410728</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>3.0632318501170901</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.03070456365092</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>3.4566744730679102</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0228582866292999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>3.86885245901638</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0161329063250499</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>4.3840749414519804</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.0091273018414699</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>4.8337236533957801</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0040832666132899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>5.4426229508196702</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.99819855884707698</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>6.11709601873536</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.99259407526020704</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>6.7540983606557301</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.98867093674939899</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>7.5035128805620603</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.98446757405924701</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>8.23419203747072</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.98194555644515502</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>9.0398126463700201</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.98026421136909403</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>9.5644028103044505</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.97970376301040796</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>10.7447306791569</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.97858286629303404</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>11.831381733021001</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.97746196957566001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>12.8430913348946</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.97718174539631597</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>13.555035128805599</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.97662129703762901</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>14.491803278688501</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.97634107285828597</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>15.503512880562001</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.97578062449959901</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>16</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.97522017614091205</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B32">
+    <sortCondition ref="A2:A32"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BD1F3D2-5535-478F-B12E-91D1BC08D30A}">
   <dimension ref="A1:B42"/>
   <sheetViews>
@@ -3864,281 +4535,4 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0FCA13A-08B5-4A81-B7EB-363371A4C292}">
-  <dimension ref="A1:B32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.91425269645608598</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1.0475651189127899</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.92619414483821205</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1.0679501698754199</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.93043143297380504</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1.0973952434881</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.93736517719568502</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1.1472253680634199</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.94699537750385199</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1.19705549263873</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.95624036979969096</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1.2468856172140399</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.96625577812018404</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1.29671574178935</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.97473035439137101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>1.3488108720271801</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.98320493066255699</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1.4009060022649999</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.99129429892141696</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>1.4484711211778001</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.99822804314329705</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1.49830124575311</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1.0055469953775</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1.55039637599094</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1.0120955315870499</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>1.6002265005662499</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1.01941448382126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>1.65005662514156</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1.0251926040061601</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>1.6998867497168699</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1.03174114021571</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>1.74971687429218</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1.0371340523882799</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>1.7995469988674899</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1.04291217257318</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>1.8810872027179999</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1.05138674884437</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>1.96715741789354</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1.0602465331278801</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>2.0509626274065602</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1.0675654853620899</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>2.14835787089467</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1.0760400616332799</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>2.2321630804077</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1.08258859784283</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>2.3227633069082598</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1.0899075500770401</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>2.4201585503963701</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1.09645608628659</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>2.5016987542468798</v>
-      </c>
-      <c r="B27" s="1">
-        <v>1.10184899845916</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>2.6013590033975</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1.10762711864406</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>2.6761041902604701</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1.1118644067796599</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>2.7848244620611502</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1.1172573189522299</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>2.90033975084937</v>
-      </c>
-      <c r="B31" s="1">
-        <v>1.1226502311247999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>3</v>
-      </c>
-      <c r="B32" s="1">
-        <v>1.1268875192604</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B32">
-    <sortCondition ref="A2:A32"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add f_h method & tests.
</commit_message>
<xml_diff>
--- a/utilityscripts/concrete/data/ccaa_t48_data.xlsx
+++ b/utilityscripts/concrete/data/ccaa_t48_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\concrete\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D546C4-0F10-4CF3-BA36-DE6476F0ABE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1F212E-7BE9-4F2B-AAFF-2B174DED09B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="14" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="17" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
   </bookViews>
   <sheets>
     <sheet name="w_fi_wheels" sheetId="1" r:id="rId1"/>
@@ -931,10 +931,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04344E26-F4EF-4CD8-95B7-38818E26435E}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,18 +953,266 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>0.38651685393258201</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>1.34999258978424</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>16</v>
+        <v>0.46741573033707601</v>
       </c>
       <c r="B3" s="1">
-        <v>1.2</v>
+        <v>1.3187026952505601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.530337078651684</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.2984560901633599</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.611235955056177</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.27391466188736</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.70112359550561598</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.2499865582132701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.79101123595505396</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.2254449576066699</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.87191011235954896</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.20274402012821</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.95280898876404296</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.1806565795822701</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1.06067415730336</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.1579551251120099</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1.22247191011235</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.1309581581305499</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1.40224719101123</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.1064148342179601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1.61797752808988</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.0861652995105799</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1.8337078651685299</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.0671427586682201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>2.1213483146067298</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0468918453160501</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>2.4089887640449401</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0333893982215401</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>2.7685393258426898</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.02172606327979</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>3.1460674157303301</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0137433652719301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>3.5056179775280798</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.00821499965533</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>4.1528089887640398</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.0014541255945399</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>4.72808988764044</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.99714861790859499</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>5.4651685393258402</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.99345350520438402</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>6.0943820224719003</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.99098745433239099</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>6.9932584269662801</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.98912973047494301</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>7.9101123595505598</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.98788515888881201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>8.8449438202247102</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.98664024264148298</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>9.8337078651685292</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.98600778934307498</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>10.5707865168539</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.98599365823395502</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>11.3258426966292</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.98597918246363803</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>12.2426966292134</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.98534810781002202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>13.051685393258399</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.98533259805610995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>14.094382022471899</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.98531260770662399</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>15.2089887640449</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.98559798717860303</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>15.999999999999901</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.98527607361963099</v>
       </c>
     </row>
   </sheetData>
@@ -1772,10 +2020,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B904222-846F-4A0A-B02A-B94E3C0047B2}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,18 +2042,274 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>0.43695525857059703</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>1.9000216743679801</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>16</v>
+        <v>0.48343986054619298</v>
       </c>
       <c r="B3" s="1">
-        <v>1.2</v>
+        <v>1.8000239801518101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.55781522370714498</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.71748798686625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.63219058686809804</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.6444758031044999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.70656595002905198</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.5746382225173601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.78094131319000404</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.5095625466921201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.91109819872167197</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.45083884415668</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1.0598489250435701</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.38735415917287</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1.20859965136548</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.33656788688746</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1.39453805926786</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.2826088560545199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1.5618826263800001</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.23817271243186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1.8036025566531</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.18897835330142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>2.1196978500871499</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.1334384770758901</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>2.3986054619407202</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.09535707368362</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>2.6961069145845298</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.0652131005413901</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>3.01220220801858</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.0430065576492</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>3.47704822777454</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.02239469485257</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>3.9790819291109698</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.0081338830322</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>4.4997094712376402</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.99863589828726496</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>5.00174317257407</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.99389889599070502</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>5.5037768739104997</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.990749195281446</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>6.1173736199883599</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.98601772686607203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>6.7495642068564603</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.98128718076423105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>7.3817547937245598</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.97814393624968998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>8.2742591516560005</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.97421995333093703</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>9.1853573503776698</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.97029689272571495</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>10.152237071469999</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.96717024985473699</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>11.007553747820999</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.96562537468987397</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>11.9186519465426</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.96408326646560405</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>12.792562463683799</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.96095201202697</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>13.5920976176641</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.96099167150881404</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>14.5403834979662</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.96103870949890902</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>15.339918651946499</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.95949106739345102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>15.999999999999901</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.95873015873015999</v>
       </c>
     </row>
   </sheetData>
@@ -2312,16 +2816,16 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D2C553-794E-4F5B-8849-B0EB72C79CE0}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2334,21 +2838,328 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>0.430698932093525</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>2.5999622635281399</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
+        <v>0.46782519716859999</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.5074356461567899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.53261416955451302</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.3812617452538301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.53261416955451302</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.3812617452538301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.606467032106774</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.2747132184259198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.68036271618738098</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.15975347289285</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.75422985258242403</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2.0504012064965602</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.846310412366853</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.96347725084003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.95667576475457705</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.8849629080813499</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1.08545437433063</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.78962452210505</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1.2417101312613601</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.69708746698616</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1.4438705665778799</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.5877239599386701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1.61846821148303</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.4923815594440799</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1.8205001822145199</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.40825170851207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1.9858055554688101</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.3381437670366101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>2.1877804308291702</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.2652288743781299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>2.40806864647839</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.1951161154807399</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>2.5732170074620901</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.1558493092575199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>2.79331966315514</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.1221851647491301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>3.01337949731986</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.09693223894591</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>3.3159135950769398</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.07167208700977</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>3.71007148964945</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.04920764560546</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>4.1867036478143298</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.0267359780682299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>4.7183043745313498</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1.00706323267746</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>5.26821844153723</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.99019262104776096</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>5.7997906205686904</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.97612735479375701</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>6.3680037540206502</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.96486261649351301</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>7.0461968461052198</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.95078450378100599</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>7.6418871269118496</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.94232109633817795</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>8.4208535490348808</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.93384163082222105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>9.0623485913278294</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.92817794842949697</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>9.8321440694636504</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.92110115560138905</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>10.5469281575189</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.91963665933199201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>11.3716993411283</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.91395691886613795</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>12.214783865026501</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.91107931216135696</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>12.9112332020288</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.91101829148346603</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>13.6626796552688</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.90814871381524997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>14.6157155901141</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.90806521183497702</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>15.5046048754986</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.90798733018029998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>16</v>
       </c>
-      <c r="B3" s="1">
-        <v>1.2</v>
+      <c r="B41" s="1">
+        <v>0.90654210359865794</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B41">
+    <sortCondition ref="A2:A41"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3906,7 +4717,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ccaa t48, simplify, add t_4 method.
</commit_message>
<xml_diff>
--- a/utilityscripts/concrete/data/ccaa_t48_data.xlsx
+++ b/utilityscripts/concrete/data/ccaa_t48_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\concrete\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1F212E-7BE9-4F2B-AAFF-2B174DED09B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1511487-5288-48DD-82C1-30B9BD974B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="17" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="18" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
   </bookViews>
   <sheets>
     <sheet name="w_fi_wheels" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="cht14_f_e" sheetId="11" r:id="rId16"/>
     <sheet name="cht14_f_s" sheetId="15" r:id="rId17"/>
     <sheet name="cht14_f_h" sheetId="20" r:id="rId18"/>
+    <sheet name="cht14_t4" sheetId="21" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
   <si>
     <t>relative_depth</t>
   </si>
@@ -89,6 +90,12 @@
   </si>
   <si>
     <t>f_h</t>
+  </si>
+  <si>
+    <t>f4</t>
+  </si>
+  <si>
+    <t>t4</t>
   </si>
 </sst>
 </file>
@@ -2818,7 +2825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D2C553-794E-4F5B-8849-B0EB72C79CE0}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B41"/>
     </sheetView>
   </sheetViews>
@@ -3160,6 +3167,400 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B41">
     <sortCondition ref="A2:A41"/>
   </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECC5E31-5DAF-46B8-8322-5E91BAFBB89A}">
+  <dimension ref="A1:B47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>36.810100605045498</v>
+      </c>
+      <c r="B2" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>38.871643058487699</v>
+      </c>
+      <c r="B3" s="1">
+        <v>579.19593468675203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>41.064148985103799</v>
+      </c>
+      <c r="B4" s="1">
+        <v>558.43311558881101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43.191314706263903</v>
+      </c>
+      <c r="B5" s="1">
+        <v>540.26435993388395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45.4820432377605</v>
+      </c>
+      <c r="B6" s="1">
+        <v>519.50093427395302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>47.118331819736497</v>
+      </c>
+      <c r="B7" s="1">
+        <v>505.65797654289901</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>49.081887553516403</v>
+      </c>
+      <c r="B8" s="1">
+        <v>489.21933787019202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>50.652741575949101</v>
+      </c>
+      <c r="B9" s="1">
+        <v>476.24133753658299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>51.9618101831648</v>
+      </c>
+      <c r="B10" s="1">
+        <v>465.85861376996797</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>53.8599313574014</v>
+      </c>
+      <c r="B11" s="1">
+        <v>450.284932494705</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>55.496267116421102</v>
+      </c>
+      <c r="B12" s="1">
+        <v>437.30652778643599</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>57.132697229528098</v>
+      </c>
+      <c r="B13" s="1">
+        <v>426.05722912373602</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>59.096418082960803</v>
+      </c>
+      <c r="B14" s="1">
+        <v>412.64452603077598</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>60.732871784589598</v>
+      </c>
+      <c r="B15" s="1">
+        <v>401.82750387946902</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>62.107469305435899</v>
+      </c>
+      <c r="B16" s="1">
+        <v>392.30892876097897</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>63.809381155129898</v>
+      </c>
+      <c r="B17" s="1">
+        <v>381.05922572361902</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>65.380376708693504</v>
+      </c>
+      <c r="B18" s="1">
+        <v>370.674884458365</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>66.362248929670798</v>
+      </c>
+      <c r="B19" s="1">
+        <v>364.18467116758097</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>67.605953742908696</v>
+      </c>
+      <c r="B20" s="1">
+        <v>355.96373433258702</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>69.242431033059304</v>
+      </c>
+      <c r="B21" s="1">
+        <v>345.57898869267302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>70.158845105971395</v>
+      </c>
+      <c r="B22" s="1">
+        <v>339.52145628794102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>71.598971540448403</v>
+      </c>
+      <c r="B23" s="1">
+        <v>330.867029817576</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>72.384469317230199</v>
+      </c>
+      <c r="B24" s="1">
+        <v>325.67485918494901</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>73.824595751707193</v>
+      </c>
+      <c r="B25" s="1">
+        <v>317.02043271458302</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>75.264722186184201</v>
+      </c>
+      <c r="B26" s="1">
+        <v>308.366006244218</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>76.443016028400507</v>
+      </c>
+      <c r="B27" s="1">
+        <v>301.44230331806199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>77.948577022420807</v>
+      </c>
+      <c r="B28" s="1">
+        <v>291.92291945025198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>79.192352601224201</v>
+      </c>
+      <c r="B29" s="1">
+        <v>284.99881214943599</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>80.174248410723294</v>
+      </c>
+      <c r="B30" s="1">
+        <v>278.94087537004401</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>81.221625956809405</v>
+      </c>
+      <c r="B31" s="1">
+        <v>272.88253421599302</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>82.399966976069393</v>
+      </c>
+      <c r="B32" s="1">
+        <v>266.82338431262099</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>83.578260818285798</v>
+      </c>
+      <c r="B33" s="1">
+        <v>259.89968138646498</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>84.691120100958798</v>
+      </c>
+      <c r="B34" s="1">
+        <v>253.840935857754</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>85.803979383631898</v>
+      </c>
+      <c r="B35" s="1">
+        <v>247.78219032904201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>86.654958897000697</v>
+      </c>
+      <c r="B36" s="1">
+        <v>242.58961532175499</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>87.898687298760393</v>
+      </c>
+      <c r="B37" s="1">
+        <v>234.800954998154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>88.880535931215803</v>
+      </c>
+      <c r="B38" s="1">
+        <v>227.87846519597801</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>90.255133452062196</v>
+      </c>
+      <c r="B39" s="1">
+        <v>218.35989007748799</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>91.498767499734598</v>
+      </c>
+      <c r="B40" s="1">
+        <v>208.84212370831699</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>92.513309823439897</v>
+      </c>
+      <c r="B41" s="1">
+        <v>201.05487869602601</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>93.658721266231794</v>
+      </c>
+      <c r="B42" s="1">
+        <v>191.53771888884501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>95.164046375033905</v>
+      </c>
+      <c r="B43" s="1">
+        <v>177.69556990711101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>96.603889747248999</v>
+      </c>
+      <c r="B44" s="1">
+        <v>163.85382530003699</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>97.258329696769493</v>
+      </c>
+      <c r="B45" s="1">
+        <v>156.93335737116001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>98.763418920353303</v>
+      </c>
+      <c r="B46" s="1">
+        <v>138.768443275501</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>100</v>
+      </c>
+      <c r="B47" s="1">
+        <v>122.33425272405201</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add ccaa_t48 t_3 method.
</commit_message>
<xml_diff>
--- a/utilityscripts/concrete/data/ccaa_t48_data.xlsx
+++ b/utilityscripts/concrete/data/ccaa_t48_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\concrete\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1511487-5288-48DD-82C1-30B9BD974B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C486DD-DE57-4D1F-9FD7-45253F626EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="18" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="11" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
   </bookViews>
   <sheets>
     <sheet name="w_fi_wheels" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,17 @@
     <sheet name="cht12_f_e" sheetId="9" r:id="rId9"/>
     <sheet name="cht12_f_s" sheetId="13" r:id="rId10"/>
     <sheet name="cht12_f_h" sheetId="18" r:id="rId11"/>
-    <sheet name="cht13_f_e_interior" sheetId="10" r:id="rId12"/>
-    <sheet name="cht13_f_e_edge" sheetId="16" r:id="rId13"/>
-    <sheet name="cht13_f_s" sheetId="14" r:id="rId14"/>
-    <sheet name="cht13_f_h" sheetId="19" r:id="rId15"/>
-    <sheet name="cht14_f_e" sheetId="11" r:id="rId16"/>
-    <sheet name="cht14_f_s" sheetId="15" r:id="rId17"/>
-    <sheet name="cht14_f_h" sheetId="20" r:id="rId18"/>
-    <sheet name="cht14_t4" sheetId="21" r:id="rId19"/>
+    <sheet name="cht12_thickness" sheetId="24" r:id="rId12"/>
+    <sheet name="cht13_f_e_interior" sheetId="10" r:id="rId13"/>
+    <sheet name="cht13_f_e_edge" sheetId="16" r:id="rId14"/>
+    <sheet name="cht13_f_s" sheetId="14" r:id="rId15"/>
+    <sheet name="cht13_f_h" sheetId="19" r:id="rId16"/>
+    <sheet name="cht13_t3_interior" sheetId="22" r:id="rId17"/>
+    <sheet name="cht13_t3_edge" sheetId="23" r:id="rId18"/>
+    <sheet name="cht14_f_e" sheetId="11" r:id="rId19"/>
+    <sheet name="cht14_f_s" sheetId="15" r:id="rId20"/>
+    <sheet name="cht14_f_h" sheetId="20" r:id="rId21"/>
+    <sheet name="cht14_t4" sheetId="21" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="19">
   <si>
     <t>relative_depth</t>
   </si>
@@ -97,6 +100,21 @@
   <si>
     <t>t4</t>
   </si>
+  <si>
+    <t>f_3</t>
+  </si>
+  <si>
+    <t>t_3</t>
+  </si>
+  <si>
+    <t>f_2</t>
+  </si>
+  <si>
+    <t>t_2</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
 </sst>
 </file>
 
@@ -134,9 +152,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1228,11 +1247,1526 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C40FADF-D801-4077-8C95-184C725DE568}">
+  <dimension ref="A1:C136"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0.325732899022801</v>
+      </c>
+      <c r="B2" s="1">
+        <v>600</v>
+      </c>
+      <c r="C2" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>0.37239117014510598</v>
+      </c>
+      <c r="B3" s="2">
+        <v>567.765042979942</v>
+      </c>
+      <c r="C3" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>0.42835442886076103</v>
+      </c>
+      <c r="B4" s="2">
+        <v>535.959885386819</v>
+      </c>
+      <c r="C4" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>0.47964769380307498</v>
+      </c>
+      <c r="B5" s="2">
+        <v>508.45272206303599</v>
+      </c>
+      <c r="C5" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>0.52627763162982399</v>
+      </c>
+      <c r="B6" s="2">
+        <v>483.52435530085899</v>
+      </c>
+      <c r="C6" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>0.61018418642108496</v>
+      </c>
+      <c r="B7" s="2">
+        <v>445.70200573065802</v>
+      </c>
+      <c r="C7" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>0.694067407910123</v>
+      </c>
+      <c r="B8" s="2">
+        <v>413.89684813753502</v>
+      </c>
+      <c r="C8" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>0.79191061078585201</v>
+      </c>
+      <c r="B9" s="2">
+        <v>382.09169054441099</v>
+      </c>
+      <c r="C9" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>0.90834712220383695</v>
+      </c>
+      <c r="B10" s="2">
+        <v>355.44412607449698</v>
+      </c>
+      <c r="C10" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>1.0573735901685399</v>
+      </c>
+      <c r="B11" s="2">
+        <v>324.498567335242</v>
+      </c>
+      <c r="C11" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>1.19706340391546</v>
+      </c>
+      <c r="B12" s="2">
+        <v>301.28939828080098</v>
+      </c>
+      <c r="C12" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>1.3693265075646499</v>
+      </c>
+      <c r="B13" s="1">
+        <v>278.08022922636002</v>
+      </c>
+      <c r="C13" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1.51364298180935</v>
+      </c>
+      <c r="B14" s="2">
+        <v>261.74785100286402</v>
+      </c>
+      <c r="C14" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>1.69053441262078</v>
+      </c>
+      <c r="B15" s="2">
+        <v>244.98567335243399</v>
+      </c>
+      <c r="C15" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>1.9186157751789601</v>
+      </c>
+      <c r="B16" s="2">
+        <v>227.36389684813599</v>
+      </c>
+      <c r="C16" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>2.10945552072597</v>
+      </c>
+      <c r="B17" s="2">
+        <v>213.610315186245</v>
+      </c>
+      <c r="C17" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>2.3282135623819098</v>
+      </c>
+      <c r="B18" s="2">
+        <v>200.286532951288</v>
+      </c>
+      <c r="C18" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>2.5236983017355898</v>
+      </c>
+      <c r="B19" s="2">
+        <v>188.681948424067</v>
+      </c>
+      <c r="C19" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>2.7377946829404198</v>
+      </c>
+      <c r="B20" s="2">
+        <v>177.50716332378099</v>
+      </c>
+      <c r="C20" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>2.9658410455452699</v>
+      </c>
+      <c r="B21" s="2">
+        <v>168.91117478509901</v>
+      </c>
+      <c r="C21" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>3.21715404379461</v>
+      </c>
+      <c r="B22" s="2">
+        <v>160.315186246417</v>
+      </c>
+      <c r="C22" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>3.5243103009196002</v>
+      </c>
+      <c r="B23" s="1">
+        <v>150.859598853867</v>
+      </c>
+      <c r="C23" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>3.6871967504043299</v>
+      </c>
+      <c r="B24" s="2">
+        <v>145.70200573065699</v>
+      </c>
+      <c r="C24" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>3.8593865208179698</v>
+      </c>
+      <c r="B25" s="2">
+        <v>141.404011461316</v>
+      </c>
+      <c r="C25" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>4.1246561671251101</v>
+      </c>
+      <c r="B26" s="2">
+        <v>133.66762177650301</v>
+      </c>
+      <c r="C26" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>4.4690423746101704</v>
+      </c>
+      <c r="B27" s="2">
+        <v>123.35243553008399</v>
+      </c>
+      <c r="C27" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>4.7668886441484704</v>
+      </c>
+      <c r="B28" s="2">
+        <v>114.756446991402</v>
+      </c>
+      <c r="C28" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>5</v>
+      </c>
+      <c r="B29" s="2">
+        <v>107.44985673352301</v>
+      </c>
+      <c r="C29" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>0.53745928338762206</v>
+      </c>
+      <c r="B30" s="1">
+        <v>600</v>
+      </c>
+      <c r="C30" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>0.60272752969662702</v>
+      </c>
+      <c r="B31" s="2">
+        <v>568.62464183380996</v>
+      </c>
+      <c r="C31" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>0.67964076047898603</v>
+      </c>
+      <c r="B32" s="2">
+        <v>534.24068767908204</v>
+      </c>
+      <c r="C32" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>0.76818397575469899</v>
+      </c>
+      <c r="B33" s="2">
+        <v>500.716332378223</v>
+      </c>
+      <c r="C33" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>0.82875389499480701</v>
+      </c>
+      <c r="B34" s="2">
+        <v>480.94555873925401</v>
+      </c>
+      <c r="C34" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>0.91261711651051103</v>
+      </c>
+      <c r="B35" s="2">
+        <v>454.29799426933999</v>
+      </c>
+      <c r="C35" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>0.99646367138177205</v>
+      </c>
+      <c r="B36" s="2">
+        <v>431.948424068767</v>
+      </c>
+      <c r="C36" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>1.1361901517464601</v>
+      </c>
+      <c r="B37" s="2">
+        <v>399.28366762177501</v>
+      </c>
+      <c r="C37" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>1.2479500027333299</v>
+      </c>
+      <c r="B38" s="2">
+        <v>378.65329512893902</v>
+      </c>
+      <c r="C38" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>1.3829798226935699</v>
+      </c>
+      <c r="B39" s="2">
+        <v>357.16332378223399</v>
+      </c>
+      <c r="C39" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>1.47609969853373</v>
+      </c>
+      <c r="B40" s="2">
+        <v>343.40974212034303</v>
+      </c>
+      <c r="C40" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>1.6018028642628399</v>
+      </c>
+      <c r="B41" s="2">
+        <v>327.07736389684698</v>
+      </c>
+      <c r="C41" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>1.73681268424975</v>
+      </c>
+      <c r="B42" s="2">
+        <v>310.74498567335098</v>
+      </c>
+      <c r="C42" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>1.82991922677436</v>
+      </c>
+      <c r="B43" s="2">
+        <v>300.42979942693302</v>
+      </c>
+      <c r="C43" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>1.94164241114345</v>
+      </c>
+      <c r="B44" s="2">
+        <v>289.25501432664601</v>
+      </c>
+      <c r="C44" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>2.1138755148326398</v>
+      </c>
+      <c r="B45" s="2">
+        <v>273.782234957019</v>
+      </c>
+      <c r="C45" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>2.23955201393064</v>
+      </c>
+      <c r="B46" s="1">
+        <v>264.326647564469</v>
+      </c>
+      <c r="C46" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>2.4257350990198598</v>
+      </c>
+      <c r="B47" s="2">
+        <v>251.432664756446</v>
+      </c>
+      <c r="C47" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>2.5514049314600902</v>
+      </c>
+      <c r="B48" s="2">
+        <v>243.69627507163199</v>
+      </c>
+      <c r="C48" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>2.6770764305647599</v>
+      </c>
+      <c r="B49" s="2">
+        <v>235.53008595988399</v>
+      </c>
+      <c r="C49" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>2.8027445963405402</v>
+      </c>
+      <c r="B50" s="2">
+        <v>228.22349570200399</v>
+      </c>
+      <c r="C50" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>2.9609910520119298</v>
+      </c>
+      <c r="B51" s="2">
+        <v>219.62750716332201</v>
+      </c>
+      <c r="C51" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>3.0820008906654799</v>
+      </c>
+      <c r="B52" s="2">
+        <v>213.610315186245</v>
+      </c>
+      <c r="C52" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>3.1937007417323402</v>
+      </c>
+      <c r="B53" s="2">
+        <v>208.45272206303599</v>
+      </c>
+      <c r="C53" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>3.3426305431592702</v>
+      </c>
+      <c r="B54" s="2">
+        <v>202.43553008595799</v>
+      </c>
+      <c r="C54" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>3.4962136717151</v>
+      </c>
+      <c r="B55" s="2">
+        <v>196.41833810888099</v>
+      </c>
+      <c r="C55" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>3.6358318188909098</v>
+      </c>
+      <c r="B56" s="2">
+        <v>191.69054441260599</v>
+      </c>
+      <c r="C56" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>3.7521799970933398</v>
+      </c>
+      <c r="B57" s="2">
+        <v>187.82234957019901</v>
+      </c>
+      <c r="C57" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>3.94764306980924</v>
+      </c>
+      <c r="B58" s="2">
+        <v>181.805157593122</v>
+      </c>
+      <c r="C58" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>4.18964441380745</v>
+      </c>
+      <c r="B59" s="2">
+        <v>174.498567335242</v>
+      </c>
+      <c r="C59" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>4.4269924306767603</v>
+      </c>
+      <c r="B60" s="2">
+        <v>167.191977077362</v>
+      </c>
+      <c r="C60" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>4.6596854537527301</v>
+      </c>
+      <c r="B61" s="2">
+        <v>160.315186246417</v>
+      </c>
+      <c r="C61" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>4.8365335512885999</v>
+      </c>
+      <c r="B62" s="2">
+        <v>154.72779369627301</v>
+      </c>
+      <c r="C62" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>5</v>
+      </c>
+      <c r="B63" s="2">
+        <v>149.570200573064</v>
+      </c>
+      <c r="C63" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>0.88180549092601201</v>
+      </c>
+      <c r="B64" s="1">
+        <v>600</v>
+      </c>
+      <c r="C64" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>0.93075709232387704</v>
+      </c>
+      <c r="B65" s="2">
+        <v>576.36103151862403</v>
+      </c>
+      <c r="C65" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>0.99601033865288202</v>
+      </c>
+      <c r="B66" s="2">
+        <v>548.85386819484199</v>
+      </c>
+      <c r="C66" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>1.0798768934974701</v>
+      </c>
+      <c r="B67" s="1">
+        <v>521.34670487105996</v>
+      </c>
+      <c r="C67" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>1.2242900342799501</v>
+      </c>
+      <c r="B68" s="2">
+        <v>480.08595988538599</v>
+      </c>
+      <c r="C68" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>1.15441346078205</v>
+      </c>
+      <c r="B69" s="2">
+        <v>499.85673352435498</v>
+      </c>
+      <c r="C69" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>1.2988099349200799</v>
+      </c>
+      <c r="B70" s="2">
+        <v>462.89398280802197</v>
+      </c>
+      <c r="C70" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>1.40592645876472</v>
+      </c>
+      <c r="B71" s="2">
+        <v>439.68481375358101</v>
+      </c>
+      <c r="C71" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>1.5130296492938</v>
+      </c>
+      <c r="B72" s="2">
+        <v>419.91404011461202</v>
+      </c>
+      <c r="C72" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>1.6666894444140701</v>
+      </c>
+      <c r="B73" s="2">
+        <v>394.12607449856603</v>
+      </c>
+      <c r="C73" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>1.8343025542632601</v>
+      </c>
+      <c r="B74" s="2">
+        <v>370.05730659025699</v>
+      </c>
+      <c r="C74" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>1.9600057199923699</v>
+      </c>
+      <c r="B75" s="2">
+        <v>353.72492836676099</v>
+      </c>
+      <c r="C75" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>2.1229388360815502</v>
+      </c>
+      <c r="B76" s="2">
+        <v>336.53295128939698</v>
+      </c>
+      <c r="C76" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>2.3417218777041602</v>
+      </c>
+      <c r="B77" s="2">
+        <v>316.76217765042901</v>
+      </c>
+      <c r="C77" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>2.5232583023222599</v>
+      </c>
+      <c r="B78" s="2">
+        <v>302.148997134669</v>
+      </c>
+      <c r="C78" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>2.6815147579803198</v>
+      </c>
+      <c r="B79" s="2">
+        <v>290.97421203438302</v>
+      </c>
+      <c r="C79" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>2.9235477686029698</v>
+      </c>
+      <c r="B80" s="2">
+        <v>275.50143266475499</v>
+      </c>
+      <c r="C80" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>3.1236875017500001</v>
+      </c>
+      <c r="B81" s="2">
+        <v>263.46704871060001</v>
+      </c>
+      <c r="C81" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>3.3284788953614699</v>
+      </c>
+      <c r="B82" s="2">
+        <v>251.86246418338001</v>
+      </c>
+      <c r="C82" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>3.5053403262129001</v>
+      </c>
+      <c r="B83" s="2">
+        <v>242.83667621776399</v>
+      </c>
+      <c r="C83" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>3.6915100779865599</v>
+      </c>
+      <c r="B84" s="2">
+        <v>233.381088825213</v>
+      </c>
+      <c r="C84" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>3.9521430638092498</v>
+      </c>
+      <c r="B85" s="2">
+        <v>221.34670487105899</v>
+      </c>
+      <c r="C85" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>4.1522694636407103</v>
+      </c>
+      <c r="B86" s="2">
+        <v>212.75071633237701</v>
+      </c>
+      <c r="C86" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>4.3523925301432902</v>
+      </c>
+      <c r="B87" s="2">
+        <v>205.014326647563</v>
+      </c>
+      <c r="C87" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>4.5571689237747703</v>
+      </c>
+      <c r="B88" s="2">
+        <v>197.27793696274901</v>
+      </c>
+      <c r="C88" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>4.81779190961079</v>
+      </c>
+      <c r="B89" s="2">
+        <v>187.82234957019901</v>
+      </c>
+      <c r="C89" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>5</v>
+      </c>
+      <c r="B90" s="2">
+        <v>181.805157593122</v>
+      </c>
+      <c r="C90" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>1.5472312703583</v>
+      </c>
+      <c r="B91" s="2">
+        <v>600</v>
+      </c>
+      <c r="C91" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>1.64271947637403</v>
+      </c>
+      <c r="B92" s="2">
+        <v>575.50143266475595</v>
+      </c>
+      <c r="C92" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>1.7358693521741899</v>
+      </c>
+      <c r="B93" s="2">
+        <v>554.01146131805103</v>
+      </c>
+      <c r="C93" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>1.84297920936105</v>
+      </c>
+      <c r="B94" s="2">
+        <v>532.521489971346</v>
+      </c>
+      <c r="C94" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>1.93611575184566</v>
+      </c>
+      <c r="B95" s="2">
+        <v>514.46991404011396</v>
+      </c>
+      <c r="C95" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>2.1503054662593799</v>
+      </c>
+      <c r="B96" s="2">
+        <v>479.22636103151802</v>
+      </c>
+      <c r="C96" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>2.2806719591040499</v>
+      </c>
+      <c r="B97" s="1">
+        <v>460.31518624641802</v>
+      </c>
+      <c r="C97" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>2.4110301186265102</v>
+      </c>
+      <c r="B98" s="2">
+        <v>443.55300859598799</v>
+      </c>
+      <c r="C98" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>2.5460382719489698</v>
+      </c>
+      <c r="B99" s="2">
+        <v>427.65042979942598</v>
+      </c>
+      <c r="C99" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>2.7415546779270898</v>
+      </c>
+      <c r="B100" s="1">
+        <v>407.87965616045801</v>
+      </c>
+      <c r="C100" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>2.7927646096471799</v>
+      </c>
+      <c r="B101" s="2">
+        <v>401.86246418337998</v>
+      </c>
+      <c r="C101" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>2.99292434276754</v>
+      </c>
+      <c r="B102" s="2">
+        <v>384.67048710601603</v>
+      </c>
+      <c r="C102" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>3.1325624899166802</v>
+      </c>
+      <c r="B103" s="2">
+        <v>374.78510028653199</v>
+      </c>
+      <c r="C103" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <v>2.8905178126429099</v>
+      </c>
+      <c r="B104" s="2">
+        <v>393.266475644698</v>
+      </c>
+      <c r="C104" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <v>3.2815072913236101</v>
+      </c>
+      <c r="B105" s="2">
+        <v>364.899713467048</v>
+      </c>
+      <c r="C105" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>3.4630303826261501</v>
+      </c>
+      <c r="B106" s="2">
+        <v>353.72492836676099</v>
+      </c>
+      <c r="C106" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>3.6771300971598699</v>
+      </c>
+      <c r="B107" s="2">
+        <v>341.69054441260602</v>
+      </c>
+      <c r="C107" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <v>3.8400298799601602</v>
+      </c>
+      <c r="B108" s="2">
+        <v>333.09455587392398</v>
+      </c>
+      <c r="C108" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>3.9889663480448698</v>
+      </c>
+      <c r="B109" s="2">
+        <v>325.35816618911099</v>
+      </c>
+      <c r="C109" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>4.2961459384720797</v>
+      </c>
+      <c r="B110" s="2">
+        <v>309.88538681948302</v>
+      </c>
+      <c r="C110" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>4.4962756716324401</v>
+      </c>
+      <c r="B111" s="2">
+        <v>300.42979942693302</v>
+      </c>
+      <c r="C111" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>4.7010587319216901</v>
+      </c>
+      <c r="B112" s="2">
+        <v>290.97421203438302</v>
+      </c>
+      <c r="C112" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>4.9058401255464998</v>
+      </c>
+      <c r="B113" s="2">
+        <v>281.948424068767</v>
+      </c>
+      <c r="C113" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>5</v>
+      </c>
+      <c r="B114" s="2">
+        <v>277.65042979942598</v>
+      </c>
+      <c r="C114" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>2.8664495114006501</v>
+      </c>
+      <c r="B115" s="2">
+        <v>600</v>
+      </c>
+      <c r="C115" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <v>2.97353436862084</v>
+      </c>
+      <c r="B116" s="2">
+        <v>584.95702005730595</v>
+      </c>
+      <c r="C116" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>3.1225175033099899</v>
+      </c>
+      <c r="B117" s="2">
+        <v>565.18624641833799</v>
+      </c>
+      <c r="C117" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>3.2901172798436198</v>
+      </c>
+      <c r="B118" s="2">
+        <v>544.55587392550103</v>
+      </c>
+      <c r="C118" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>3.4297770936305398</v>
+      </c>
+      <c r="B119" s="2">
+        <v>529.083094555873</v>
+      </c>
+      <c r="C119" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>3.6532234623687199</v>
+      </c>
+      <c r="B120" s="2">
+        <v>506.73352435530001</v>
+      </c>
+      <c r="C120" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>3.7975299366267499</v>
+      </c>
+      <c r="B121" s="2">
+        <v>492.97994269340899</v>
+      </c>
+      <c r="C121" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>3.9464897380136801</v>
+      </c>
+      <c r="B122" s="2">
+        <v>479.22636103151802</v>
+      </c>
+      <c r="C122" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>4.0675179099761198</v>
+      </c>
+      <c r="B123" s="1">
+        <v>468.48137535816602</v>
+      </c>
+      <c r="C123" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>4.2350893532141898</v>
+      </c>
+      <c r="B124" s="1">
+        <v>455.15759312320898</v>
+      </c>
+      <c r="C124" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>4.4259290987612001</v>
+      </c>
+      <c r="B125" s="2">
+        <v>441.404011461317</v>
+      </c>
+      <c r="C125" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>4.6865854178861097</v>
+      </c>
+      <c r="B126" s="2">
+        <v>423.35243553008502</v>
+      </c>
+      <c r="C126" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <v>4.8587985216019698</v>
+      </c>
+      <c r="B127" s="2">
+        <v>413.03724928366699</v>
+      </c>
+      <c r="C127" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>5</v>
+      </c>
+      <c r="B128" s="2">
+        <v>405.30085959885298</v>
+      </c>
+      <c r="C128" s="2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
+        <v>3.8134015821312199</v>
+      </c>
+      <c r="B129" s="2">
+        <v>600</v>
+      </c>
+      <c r="C129" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
+        <v>3.9833163555781899</v>
+      </c>
+      <c r="B130" s="2">
+        <v>582.37822349570195</v>
+      </c>
+      <c r="C130" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
+        <v>4.1834794220274301</v>
+      </c>
+      <c r="B131" s="1">
+        <v>564.32664756447002</v>
+      </c>
+      <c r="C131" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <v>4.33243255675659</v>
+      </c>
+      <c r="B132" s="2">
+        <v>552.29226361031499</v>
+      </c>
+      <c r="C132" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <v>4.5186189751747001</v>
+      </c>
+      <c r="B133" s="2">
+        <v>538.53868194842403</v>
+      </c>
+      <c r="C133" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>4.7327320230239698</v>
+      </c>
+      <c r="B134" s="2">
+        <v>523.065902578796</v>
+      </c>
+      <c r="C134" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
+        <v>4.8584051887930801</v>
+      </c>
+      <c r="B135" s="2">
+        <v>514.46991404011396</v>
+      </c>
+      <c r="C135" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
+        <v>5</v>
+      </c>
+      <c r="B136" s="2">
+        <v>505.444126074498</v>
+      </c>
+      <c r="C136" s="1">
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2756CE3D-CA0B-49BC-927E-820826FB3317}">
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,12 +3043,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1189659-55E8-4E76-8A86-E883731015EF}">
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B31"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,7 +3313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA43ABBA-596A-44DB-ACD5-DD0354E71F86}">
   <dimension ref="A1:B28"/>
   <sheetViews>
@@ -2025,7 +3559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B904222-846F-4A0A-B02A-B94E3C0047B2}">
   <dimension ref="A1:B35"/>
   <sheetViews>
@@ -2324,7 +3858,765 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E07D5958-068D-41A7-95B3-DC18AFCF919D}">
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>14.7882136279925</v>
+      </c>
+      <c r="B2" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>15.8931860036831</v>
+      </c>
+      <c r="B3" s="1">
+        <v>575.68198738293904</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>17.5874769797421</v>
+      </c>
+      <c r="B4" s="1">
+        <v>541.62140981936398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>18.6924493554327</v>
+      </c>
+      <c r="B5" s="1">
+        <v>520.33305904941005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>19.539594843462101</v>
+      </c>
+      <c r="B6" s="1">
+        <v>505.00489792719702</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>20.534069981583698</v>
+      </c>
+      <c r="B7" s="1">
+        <v>488.82410563849402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>21.7863720073663</v>
+      </c>
+      <c r="B8" s="1">
+        <v>468.385251361624</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>23.112338858195098</v>
+      </c>
+      <c r="B9" s="1">
+        <v>448.79667724618901</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>24.069981583793599</v>
+      </c>
+      <c r="B10" s="1">
+        <v>435.16946828102402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>25.248618784530201</v>
+      </c>
+      <c r="B11" s="1">
+        <v>420.26331256612201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>26.795580110496999</v>
+      </c>
+      <c r="B12" s="1">
+        <v>401.94898319031398</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>28.121546961325802</v>
+      </c>
+      <c r="B13" s="1">
+        <v>387.04126013870899</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>29.594843462246601</v>
+      </c>
+      <c r="B14" s="1">
+        <v>371.280905920615</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>31.215469613259401</v>
+      </c>
+      <c r="B15" s="1">
+        <v>355.518984365817</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>32.909760589318402</v>
+      </c>
+      <c r="B16" s="1">
+        <v>340.18181105756099</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>34.309392265193097</v>
+      </c>
+      <c r="B17" s="1">
+        <v>327.82649582696598</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>36.0773480662981</v>
+      </c>
+      <c r="B18" s="1">
+        <v>314.19066650993301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>37.329650092080698</v>
+      </c>
+      <c r="B19" s="1">
+        <v>304.81564202029801</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>38.729281767955499</v>
+      </c>
+      <c r="B20" s="1">
+        <v>294.587986364171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>40.4235727440144</v>
+      </c>
+      <c r="B21" s="1">
+        <v>282.65506837506399</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>41.7495395948431</v>
+      </c>
+      <c r="B22" s="1">
+        <v>274.13032404686402</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43.517495395948103</v>
+      </c>
+      <c r="B23" s="1">
+        <v>263.047686219193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>45.359116022099101</v>
+      </c>
+      <c r="B24" s="1">
+        <v>252.815328552957</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>47.127071823203998</v>
+      </c>
+      <c r="B25" s="1">
+        <v>243.43481838485999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>48.674033149170903</v>
+      </c>
+      <c r="B26" s="1">
+        <v>234.90772305160499</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>50.0368324125226</v>
+      </c>
+      <c r="B27" s="1">
+        <v>228.08471454880399</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>52.799263351749303</v>
+      </c>
+      <c r="B28" s="1">
+        <v>218.70851455664001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>55.598526703498798</v>
+      </c>
+      <c r="B29" s="1">
+        <v>209.757454645195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>58.987108655616701</v>
+      </c>
+      <c r="B30" s="1">
+        <v>199.95219623055601</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>62.965009208102899</v>
+      </c>
+      <c r="B31" s="1">
+        <v>189.71827122761701</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>66.648250460404896</v>
+      </c>
+      <c r="B32" s="1">
+        <v>181.18804122095599</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>71.362799263351505</v>
+      </c>
+      <c r="B33" s="1">
+        <v>170.95019787626001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>75.193370165745705</v>
+      </c>
+      <c r="B34" s="1">
+        <v>163.27024803103399</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>78.139963167587297</v>
+      </c>
+      <c r="B35" s="1">
+        <v>157.722659770386</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>82.265193370165605</v>
+      </c>
+      <c r="B36" s="1">
+        <v>150.892206418245</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>86.537753222835903</v>
+      </c>
+      <c r="B37" s="1">
+        <v>144.06096939775199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>90.368324125230004</v>
+      </c>
+      <c r="B38" s="1">
+        <v>138.508679126994</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>94.788213627992505</v>
+      </c>
+      <c r="B39" s="1">
+        <v>132.10219035304399</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>98.618784530386606</v>
+      </c>
+      <c r="B40" s="1">
+        <v>127.400963912073</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>103.03867403314899</v>
+      </c>
+      <c r="B41" s="1">
+        <v>122.271070882803</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>105.69060773480599</v>
+      </c>
+      <c r="B42" s="1">
+        <v>118.85270953332601</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>108.93186003683201</v>
+      </c>
+      <c r="B43" s="1">
+        <v>115.431213510443</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>113.05709023941</v>
+      </c>
+      <c r="B44" s="1">
+        <v>111.153951647664</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>118.066298342541</v>
+      </c>
+      <c r="B45" s="1">
+        <v>106.87198777477499</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>123.075506445672</v>
+      </c>
+      <c r="B46" s="1">
+        <v>102.590023901886</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>127.348066298342</v>
+      </c>
+      <c r="B47" s="1">
+        <v>100.014106030329</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>130</v>
+      </c>
+      <c r="B48" s="1">
+        <v>99.148936170214199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052C11E2-875D-4CFB-A1E2-78443E489239}">
+  <dimension ref="A1:B43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>27.127071823204201</v>
+      </c>
+      <c r="B2" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>29.373848987108399</v>
+      </c>
+      <c r="B3" s="1">
+        <v>579.79389522354097</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>31.0681399631674</v>
+      </c>
+      <c r="B4" s="1">
+        <v>564.45672191528502</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>32.246777163904</v>
+      </c>
+      <c r="B5" s="1">
+        <v>554.23141726421295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>33.867403314916899</v>
+      </c>
+      <c r="B6" s="1">
+        <v>539.74609145409602</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>35.561694290975801</v>
+      </c>
+      <c r="B7" s="1">
+        <v>525.25998197562797</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>36.813996316758498</v>
+      </c>
+      <c r="B8" s="1">
+        <v>515.03389365620399</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>37.918968692449099</v>
+      </c>
+      <c r="B9" s="1">
+        <v>505.66043650327202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>39.465930018415897</v>
+      </c>
+      <c r="B10" s="1">
+        <v>492.45249010618699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>41.160220994474798</v>
+      </c>
+      <c r="B11" s="1">
+        <v>478.39191254261198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>42.8545119705337</v>
+      </c>
+      <c r="B12" s="1">
+        <v>464.75686689393001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44.033149171270402</v>
+      </c>
+      <c r="B13" s="1">
+        <v>455.38262607264602</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45.432780847145096</v>
+      </c>
+      <c r="B14" s="1">
+        <v>444.30390658673201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>46.906077348065899</v>
+      </c>
+      <c r="B15" s="1">
+        <v>432.79887151757401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>47.937384898710498</v>
+      </c>
+      <c r="B16" s="1">
+        <v>425.553857607461</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>49.410681399631301</v>
+      </c>
+      <c r="B17" s="1">
+        <v>414.47435445319502</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>49.963167587476597</v>
+      </c>
+      <c r="B18" s="1">
+        <v>410.21315779162302</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>51.178637200736397</v>
+      </c>
+      <c r="B19" s="1">
+        <v>403.39798597233698</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>53.093922651933497</v>
+      </c>
+      <c r="B20" s="1">
+        <v>394.02609615610697</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>56.924493554327597</v>
+      </c>
+      <c r="B21" s="1">
+        <v>375.70784843854102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>60.460405156537497</v>
+      </c>
+      <c r="B22" s="1">
+        <v>359.51882763214599</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>62.670349907918698</v>
+      </c>
+      <c r="B23" s="1">
+        <v>349.71983856432001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>65.616942909760397</v>
+      </c>
+      <c r="B24" s="1">
+        <v>336.93820775047999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>67.974217311233701</v>
+      </c>
+      <c r="B25" s="1">
+        <v>327.563966929196</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>71.362799263351505</v>
+      </c>
+      <c r="B26" s="1">
+        <v>313.92892128051398</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>73.278084714548598</v>
+      </c>
+      <c r="B27" s="1">
+        <v>306.25915912385898</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>76.0773480662981</v>
+      </c>
+      <c r="B28" s="1">
+        <v>295.60597155283898</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>79.613259668508107</v>
+      </c>
+      <c r="B29" s="1">
+        <v>283.24673798048701</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>82.265193370165605</v>
+      </c>
+      <c r="B30" s="1">
+        <v>273.44539790760598</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>87.127071823204204</v>
+      </c>
+      <c r="B31" s="1">
+        <v>256.82379217115403</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>90.073664825045896</v>
+      </c>
+      <c r="B32" s="1">
+        <v>247.446416676463</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>92.578268876611304</v>
+      </c>
+      <c r="B33" s="1">
+        <v>239.773519846402</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>95.966850828729093</v>
+      </c>
+      <c r="B34" s="1">
+        <v>229.542729516869</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>99.208103130754907</v>
+      </c>
+      <c r="B35" s="1">
+        <v>220.58931860036901</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>103.03867403314899</v>
+      </c>
+      <c r="B36" s="1">
+        <v>209.930645350888</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>107.163904235727</v>
+      </c>
+      <c r="B37" s="1">
+        <v>199.69593667959799</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>110.847145488029</v>
+      </c>
+      <c r="B38" s="1">
+        <v>190.31464284315001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>114.235727440147</v>
+      </c>
+      <c r="B39" s="1">
+        <v>183.48810783276599</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>117.918968692449</v>
+      </c>
+      <c r="B40" s="1">
+        <v>175.808941655892</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>121.602209944751</v>
+      </c>
+      <c r="B41" s="1">
+        <v>168.12977547901801</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>125.580110497237</v>
+      </c>
+      <c r="B42" s="1">
+        <v>161.30010579522801</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>130</v>
+      </c>
+      <c r="B43" s="1">
+        <v>154.468085106384</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4FF09A-ECDC-4607-B00C-BBA37F8F7346}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -2538,1029 +4830,6 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B25">
     <sortCondition ref="A2:A25"/>
   </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D80BD14-9AEF-4A12-BFA1-6D4BF756A2E8}">
-  <dimension ref="A1:B33"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0.98879551820728195</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1.0138235722423501</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1.6415137614678801</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1.03609976100531</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1.59885321100917</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1.0695461670906801</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1.5451834862385301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1.10582367503576</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1.5011467889908201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1.1644715990371599</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1.4447247706422</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1.22314950445009</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1.39793577981651</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1.30420639203693</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1.34151376146788</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>1.3797038693153001</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1.29885321100917</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1.48319541884031</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1.2506880733944901</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>1.59789573321683</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1.2038990825688001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1.7098206254979</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1.1653669724770599</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1.8441501983056201</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1.12545871559633</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>1.9952907768612</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1.0869266055045801</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>2.1296503310804402</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1.05665137614678</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>2.2612258970866601</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1.0318807339449501</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>2.4404033784767698</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1.0016055045871499</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>2.6307981908359599</v>
-      </c>
-      <c r="B19" s="1">
-        <v>0.97545871559632902</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>2.7820072983321702</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0.95894495412843905</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>2.9220162070944502</v>
-      </c>
-      <c r="B21" s="1">
-        <v>0.94380733944953998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>3.0956342781760999</v>
-      </c>
-      <c r="B22" s="1">
-        <v>0.92729357798165102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>3.27766427671986</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0.91353211009174196</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>3.4765074225408799</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0.90183486238531996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>3.6501511919752598</v>
-      </c>
-      <c r="B25" s="1">
-        <v>0.89357798165137503</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>3.8406016840987101</v>
-      </c>
-      <c r="B26" s="1">
-        <v>0.88532110091742999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>4.0198584020764203</v>
-      </c>
-      <c r="B27" s="1">
-        <v>0.88050458715596303</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>4.1823191050120299</v>
-      </c>
-      <c r="B28" s="1">
-        <v>0.87912844036697202</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>4.39520425907366</v>
-      </c>
-      <c r="B29" s="1">
-        <v>0.87912844036697202</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>4.5800889163004603</v>
-      </c>
-      <c r="B30" s="1">
-        <v>0.88256880733944898</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>4.7649842811742404</v>
-      </c>
-      <c r="B31" s="1">
-        <v>0.88944954128440301</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>4.8938636616726203</v>
-      </c>
-      <c r="B32" s="1">
-        <v>0.898394495412843</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>4.99753509966677</v>
-      </c>
-      <c r="B33" s="1">
-        <v>0.90802752293577904</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D2C553-794E-4F5B-8849-B0EB72C79CE0}">
-  <dimension ref="A1:B41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0.430698932093525</v>
-      </c>
-      <c r="B2" s="1">
-        <v>2.5999622635281399</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>0.46782519716859999</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2.5074356461567899</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>0.53261416955451302</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2.3812617452538301</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.53261416955451302</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2.3812617452538301</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0.606467032106774</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2.2747132184259198</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0.68036271618738098</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2.15975347289285</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0.75422985258242403</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2.0504012064965602</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>0.846310412366853</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1.96347725084003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0.95667576475457705</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1.8849629080813499</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1.08545437433063</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1.78962452210505</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>1.2417101312613601</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1.69708746698616</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1.4438705665778799</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1.5877239599386701</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1.61846821148303</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1.4923815594440799</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>1.8205001822145199</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1.40825170851207</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>1.9858055554688101</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1.3381437670366101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>2.1877804308291702</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1.2652288743781299</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>2.40806864647839</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1.1951161154807399</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>2.5732170074620901</v>
-      </c>
-      <c r="B19" s="1">
-        <v>1.1558493092575199</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>2.79331966315514</v>
-      </c>
-      <c r="B20" s="1">
-        <v>1.1221851647491301</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>3.01337949731986</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1.09693223894591</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>3.3159135950769398</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1.07167208700977</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>3.71007148964945</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1.04920764560546</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>4.1867036478143298</v>
-      </c>
-      <c r="B24" s="1">
-        <v>1.0267359780682299</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>4.7183043745313498</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1.00706323267746</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>5.26821844153723</v>
-      </c>
-      <c r="B26" s="1">
-        <v>0.99019262104776096</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>5.7997906205686904</v>
-      </c>
-      <c r="B27" s="1">
-        <v>0.97612735479375701</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>6.3680037540206502</v>
-      </c>
-      <c r="B28" s="1">
-        <v>0.96486261649351301</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>7.0461968461052198</v>
-      </c>
-      <c r="B29" s="1">
-        <v>0.95078450378100599</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>7.6418871269118496</v>
-      </c>
-      <c r="B30" s="1">
-        <v>0.94232109633817795</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>8.4208535490348808</v>
-      </c>
-      <c r="B31" s="1">
-        <v>0.93384163082222105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>9.0623485913278294</v>
-      </c>
-      <c r="B32" s="1">
-        <v>0.92817794842949697</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>9.8321440694636504</v>
-      </c>
-      <c r="B33" s="1">
-        <v>0.92110115560138905</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>10.5469281575189</v>
-      </c>
-      <c r="B34" s="1">
-        <v>0.91963665933199201</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>11.3716993411283</v>
-      </c>
-      <c r="B35" s="1">
-        <v>0.91395691886613795</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>12.214783865026501</v>
-      </c>
-      <c r="B36" s="1">
-        <v>0.91107931216135696</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>12.9112332020288</v>
-      </c>
-      <c r="B37" s="1">
-        <v>0.91101829148346603</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>13.6626796552688</v>
-      </c>
-      <c r="B38" s="1">
-        <v>0.90814871381524997</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>14.6157155901141</v>
-      </c>
-      <c r="B39" s="1">
-        <v>0.90806521183497702</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>15.5046048754986</v>
-      </c>
-      <c r="B40" s="1">
-        <v>0.90798733018029998</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>16</v>
-      </c>
-      <c r="B41" s="1">
-        <v>0.90654210359865794</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B41">
-    <sortCondition ref="A2:A41"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECC5E31-5DAF-46B8-8322-5E91BAFBB89A}">
-  <dimension ref="A1:B47"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>36.810100605045498</v>
-      </c>
-      <c r="B2" s="1">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>38.871643058487699</v>
-      </c>
-      <c r="B3" s="1">
-        <v>579.19593468675203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>41.064148985103799</v>
-      </c>
-      <c r="B4" s="1">
-        <v>558.43311558881101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>43.191314706263903</v>
-      </c>
-      <c r="B5" s="1">
-        <v>540.26435993388395</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>45.4820432377605</v>
-      </c>
-      <c r="B6" s="1">
-        <v>519.50093427395302</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>47.118331819736497</v>
-      </c>
-      <c r="B7" s="1">
-        <v>505.65797654289901</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>49.081887553516403</v>
-      </c>
-      <c r="B8" s="1">
-        <v>489.21933787019202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>50.652741575949101</v>
-      </c>
-      <c r="B9" s="1">
-        <v>476.24133753658299</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>51.9618101831648</v>
-      </c>
-      <c r="B10" s="1">
-        <v>465.85861376996797</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>53.8599313574014</v>
-      </c>
-      <c r="B11" s="1">
-        <v>450.284932494705</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>55.496267116421102</v>
-      </c>
-      <c r="B12" s="1">
-        <v>437.30652778643599</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>57.132697229528098</v>
-      </c>
-      <c r="B13" s="1">
-        <v>426.05722912373602</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>59.096418082960803</v>
-      </c>
-      <c r="B14" s="1">
-        <v>412.64452603077598</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>60.732871784589598</v>
-      </c>
-      <c r="B15" s="1">
-        <v>401.82750387946902</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>62.107469305435899</v>
-      </c>
-      <c r="B16" s="1">
-        <v>392.30892876097897</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>63.809381155129898</v>
-      </c>
-      <c r="B17" s="1">
-        <v>381.05922572361902</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>65.380376708693504</v>
-      </c>
-      <c r="B18" s="1">
-        <v>370.674884458365</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>66.362248929670798</v>
-      </c>
-      <c r="B19" s="1">
-        <v>364.18467116758097</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>67.605953742908696</v>
-      </c>
-      <c r="B20" s="1">
-        <v>355.96373433258702</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>69.242431033059304</v>
-      </c>
-      <c r="B21" s="1">
-        <v>345.57898869267302</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>70.158845105971395</v>
-      </c>
-      <c r="B22" s="1">
-        <v>339.52145628794102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>71.598971540448403</v>
-      </c>
-      <c r="B23" s="1">
-        <v>330.867029817576</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>72.384469317230199</v>
-      </c>
-      <c r="B24" s="1">
-        <v>325.67485918494901</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>73.824595751707193</v>
-      </c>
-      <c r="B25" s="1">
-        <v>317.02043271458302</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>75.264722186184201</v>
-      </c>
-      <c r="B26" s="1">
-        <v>308.366006244218</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>76.443016028400507</v>
-      </c>
-      <c r="B27" s="1">
-        <v>301.44230331806199</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>77.948577022420807</v>
-      </c>
-      <c r="B28" s="1">
-        <v>291.92291945025198</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>79.192352601224201</v>
-      </c>
-      <c r="B29" s="1">
-        <v>284.99881214943599</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>80.174248410723294</v>
-      </c>
-      <c r="B30" s="1">
-        <v>278.94087537004401</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>81.221625956809405</v>
-      </c>
-      <c r="B31" s="1">
-        <v>272.88253421599302</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>82.399966976069393</v>
-      </c>
-      <c r="B32" s="1">
-        <v>266.82338431262099</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>83.578260818285798</v>
-      </c>
-      <c r="B33" s="1">
-        <v>259.89968138646498</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>84.691120100958798</v>
-      </c>
-      <c r="B34" s="1">
-        <v>253.840935857754</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>85.803979383631898</v>
-      </c>
-      <c r="B35" s="1">
-        <v>247.78219032904201</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>86.654958897000697</v>
-      </c>
-      <c r="B36" s="1">
-        <v>242.58961532175499</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>87.898687298760393</v>
-      </c>
-      <c r="B37" s="1">
-        <v>234.800954998154</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>88.880535931215803</v>
-      </c>
-      <c r="B38" s="1">
-        <v>227.87846519597801</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>90.255133452062196</v>
-      </c>
-      <c r="B39" s="1">
-        <v>218.35989007748799</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>91.498767499734598</v>
-      </c>
-      <c r="B40" s="1">
-        <v>208.84212370831699</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>92.513309823439897</v>
-      </c>
-      <c r="B41" s="1">
-        <v>201.05487869602601</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>93.658721266231794</v>
-      </c>
-      <c r="B42" s="1">
-        <v>191.53771888884501</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>95.164046375033905</v>
-      </c>
-      <c r="B43" s="1">
-        <v>177.69556990711101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>96.603889747248999</v>
-      </c>
-      <c r="B44" s="1">
-        <v>163.85382530003699</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>97.258329696769493</v>
-      </c>
-      <c r="B45" s="1">
-        <v>156.93335737116001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>98.763418920353303</v>
-      </c>
-      <c r="B46" s="1">
-        <v>138.768443275501</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>100</v>
-      </c>
-      <c r="B47" s="1">
-        <v>122.33425272405201</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3735,6 +5004,1029 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B19">
     <sortCondition ref="A2:A19"/>
   </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D80BD14-9AEF-4A12-BFA1-6D4BF756A2E8}">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0.98879551820728195</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1.0138235722423501</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.6415137614678801</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1.03609976100531</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.59885321100917</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1.0695461670906801</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.5451834862385301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1.10582367503576</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.5011467889908201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1.1644715990371599</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.4447247706422</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1.22314950445009</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.39793577981651</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1.30420639203693</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.34151376146788</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1.3797038693153001</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.29885321100917</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1.48319541884031</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.2506880733944901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1.59789573321683</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.2038990825688001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1.7098206254979</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.1653669724770599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1.8441501983056201</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.12545871559633</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1.9952907768612</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.0869266055045801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>2.1296503310804402</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.05665137614678</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>2.2612258970866601</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.0318807339449501</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>2.4404033784767698</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.0016055045871499</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>2.6307981908359599</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.97545871559632902</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>2.7820072983321702</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.95894495412843905</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>2.9220162070944502</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.94380733944953998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>3.0956342781760999</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.92729357798165102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>3.27766427671986</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.91353211009174196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>3.4765074225408799</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.90183486238531996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>3.6501511919752598</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.89357798165137503</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>3.8406016840987101</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.88532110091742999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>4.0198584020764203</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.88050458715596303</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>4.1823191050120299</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.87912844036697202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>4.39520425907366</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.87912844036697202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>4.5800889163004603</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.88256880733944898</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>4.7649842811742404</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.88944954128440301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>4.8938636616726203</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.898394495412843</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>4.99753509966677</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.90802752293577904</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D2C553-794E-4F5B-8849-B0EB72C79CE0}">
+  <dimension ref="A1:B41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0.430698932093525</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.5999622635281399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>0.46782519716859999</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.5074356461567899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.53261416955451302</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.3812617452538301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>0.53261416955451302</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.3812617452538301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0.606467032106774</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.2747132184259198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.68036271618738098</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2.15975347289285</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>0.75422985258242403</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2.0504012064965602</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>0.846310412366853</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.96347725084003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0.95667576475457705</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.8849629080813499</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1.08545437433063</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.78962452210505</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1.2417101312613601</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.69708746698616</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1.4438705665778799</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.5877239599386701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1.61846821148303</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.4923815594440799</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1.8205001822145199</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.40825170851207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1.9858055554688101</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.3381437670366101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>2.1877804308291702</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.2652288743781299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>2.40806864647839</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.1951161154807399</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>2.5732170074620901</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1.1558493092575199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>2.79331966315514</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1.1221851647491301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>3.01337949731986</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1.09693223894591</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>3.3159135950769398</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1.07167208700977</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>3.71007148964945</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1.04920764560546</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>4.1867036478143298</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.0267359780682299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>4.7183043745313498</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1.00706323267746</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>5.26821844153723</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.99019262104776096</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>5.7997906205686904</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.97612735479375701</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>6.3680037540206502</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.96486261649351301</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>7.0461968461052198</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.95078450378100599</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>7.6418871269118496</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.94232109633817795</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>8.4208535490348808</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.93384163082222105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>9.0623485913278294</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.92817794842949697</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>9.8321440694636504</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.92110115560138905</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>10.5469281575189</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.91963665933199201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>11.3716993411283</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.91395691886613795</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>12.214783865026501</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.91107931216135696</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>12.9112332020288</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.91101829148346603</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>13.6626796552688</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.90814871381524997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>14.6157155901141</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.90806521183497702</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>15.5046048754986</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.90798733018029998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>16</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.90654210359865794</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B41">
+    <sortCondition ref="A2:A41"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECC5E31-5DAF-46B8-8322-5E91BAFBB89A}">
+  <dimension ref="A1:B47"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>36.810100605045498</v>
+      </c>
+      <c r="B2" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>38.871643058487699</v>
+      </c>
+      <c r="B3" s="1">
+        <v>579.19593468675203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>41.064148985103799</v>
+      </c>
+      <c r="B4" s="1">
+        <v>558.43311558881101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43.191314706263903</v>
+      </c>
+      <c r="B5" s="1">
+        <v>540.26435993388395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45.4820432377605</v>
+      </c>
+      <c r="B6" s="1">
+        <v>519.50093427395302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>47.118331819736497</v>
+      </c>
+      <c r="B7" s="1">
+        <v>505.65797654289901</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>49.081887553516403</v>
+      </c>
+      <c r="B8" s="1">
+        <v>489.21933787019202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>50.652741575949101</v>
+      </c>
+      <c r="B9" s="1">
+        <v>476.24133753658299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>51.9618101831648</v>
+      </c>
+      <c r="B10" s="1">
+        <v>465.85861376996797</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>53.8599313574014</v>
+      </c>
+      <c r="B11" s="1">
+        <v>450.284932494705</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>55.496267116421102</v>
+      </c>
+      <c r="B12" s="1">
+        <v>437.30652778643599</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>57.132697229528098</v>
+      </c>
+      <c r="B13" s="1">
+        <v>426.05722912373602</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>59.096418082960803</v>
+      </c>
+      <c r="B14" s="1">
+        <v>412.64452603077598</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>60.732871784589598</v>
+      </c>
+      <c r="B15" s="1">
+        <v>401.82750387946902</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>62.107469305435899</v>
+      </c>
+      <c r="B16" s="1">
+        <v>392.30892876097897</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>63.809381155129898</v>
+      </c>
+      <c r="B17" s="1">
+        <v>381.05922572361902</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>65.380376708693504</v>
+      </c>
+      <c r="B18" s="1">
+        <v>370.674884458365</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>66.362248929670798</v>
+      </c>
+      <c r="B19" s="1">
+        <v>364.18467116758097</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>67.605953742908696</v>
+      </c>
+      <c r="B20" s="1">
+        <v>355.96373433258702</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>69.242431033059304</v>
+      </c>
+      <c r="B21" s="1">
+        <v>345.57898869267302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>70.158845105971395</v>
+      </c>
+      <c r="B22" s="1">
+        <v>339.52145628794102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>71.598971540448403</v>
+      </c>
+      <c r="B23" s="1">
+        <v>330.867029817576</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>72.384469317230199</v>
+      </c>
+      <c r="B24" s="1">
+        <v>325.67485918494901</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>73.824595751707193</v>
+      </c>
+      <c r="B25" s="1">
+        <v>317.02043271458302</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>75.264722186184201</v>
+      </c>
+      <c r="B26" s="1">
+        <v>308.366006244218</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>76.443016028400507</v>
+      </c>
+      <c r="B27" s="1">
+        <v>301.44230331806199</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>77.948577022420807</v>
+      </c>
+      <c r="B28" s="1">
+        <v>291.92291945025198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>79.192352601224201</v>
+      </c>
+      <c r="B29" s="1">
+        <v>284.99881214943599</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>80.174248410723294</v>
+      </c>
+      <c r="B30" s="1">
+        <v>278.94087537004401</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>81.221625956809405</v>
+      </c>
+      <c r="B31" s="1">
+        <v>272.88253421599302</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>82.399966976069393</v>
+      </c>
+      <c r="B32" s="1">
+        <v>266.82338431262099</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>83.578260818285798</v>
+      </c>
+      <c r="B33" s="1">
+        <v>259.89968138646498</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>84.691120100958798</v>
+      </c>
+      <c r="B34" s="1">
+        <v>253.840935857754</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>85.803979383631898</v>
+      </c>
+      <c r="B35" s="1">
+        <v>247.78219032904201</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>86.654958897000697</v>
+      </c>
+      <c r="B36" s="1">
+        <v>242.58961532175499</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>87.898687298760393</v>
+      </c>
+      <c r="B37" s="1">
+        <v>234.800954998154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>88.880535931215803</v>
+      </c>
+      <c r="B38" s="1">
+        <v>227.87846519597801</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>90.255133452062196</v>
+      </c>
+      <c r="B39" s="1">
+        <v>218.35989007748799</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>91.498767499734598</v>
+      </c>
+      <c r="B40" s="1">
+        <v>208.84212370831699</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>92.513309823439897</v>
+      </c>
+      <c r="B41" s="1">
+        <v>201.05487869602601</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>93.658721266231794</v>
+      </c>
+      <c r="B42" s="1">
+        <v>191.53771888884501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>95.164046375033905</v>
+      </c>
+      <c r="B43" s="1">
+        <v>177.69556990711101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>96.603889747248999</v>
+      </c>
+      <c r="B44" s="1">
+        <v>163.85382530003699</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>97.258329696769493</v>
+      </c>
+      <c r="B45" s="1">
+        <v>156.93335737116001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>98.763418920353303</v>
+      </c>
+      <c r="B46" s="1">
+        <v>138.768443275501</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>100</v>
+      </c>
+      <c r="B47" s="1">
+        <v>122.33425272405201</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add t_12 method, data & tests.
</commit_message>
<xml_diff>
--- a/utilityscripts/concrete/data/ccaa_t48_data.xlsx
+++ b/utilityscripts/concrete/data/ccaa_t48_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\concrete\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69A25B8-2724-440E-9F69-E67CA6EF58D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E456A02-7FEC-413A-A5D8-8AC2A7F40885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="7" activeTab="12" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="7" activeTab="8" xr2:uid="{66767DF0-AC09-4DC7-8E07-8A09C004970D}"/>
   </bookViews>
   <sheets>
     <sheet name="w_fi_wheels" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
   <si>
     <t>relative_depth</t>
   </si>
@@ -108,19 +108,13 @@
     <t>t_3</t>
   </si>
   <si>
-    <t>f_2</t>
-  </si>
-  <si>
-    <t>t_2</t>
-  </si>
-  <si>
     <t>p</t>
   </si>
   <si>
-    <t>t_1</t>
+    <t>f</t>
   </si>
   <si>
-    <t>f_1</t>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -1615,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C40FADF-D801-4077-8C95-184C725DE568}">
   <dimension ref="A1:C137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,13 +1621,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -8063,21 +8057,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD42F23B-2E5F-4C28-932C-57FA12225DB9}">
   <dimension ref="A1:C283"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>